<commit_message>
finished coding for cs351
</commit_message>
<xml_diff>
--- a/cs351/proj4/deliverables/charts.xlsx
+++ b/cs351/proj4/deliverables/charts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>V=10</t>
   </si>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +61,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -99,13 +105,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -177,7 +187,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1283,11 +1292,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="224061200"/>
-        <c:axId val="224068480"/>
+        <c:axId val="221453472"/>
+        <c:axId val="221454592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="224061200"/>
+        <c:axId val="221453472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1347,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1405,12 +1413,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224068480"/>
+        <c:crossAx val="221454592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="224068480"/>
+        <c:axId val="221454592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1456,7 +1464,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1523,7 +1530,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224061200"/>
+        <c:crossAx val="221453472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1537,7 +1544,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1674,16 +1680,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -1778,73 +1781,19 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$11</c:f>
+              <c:f>Sheet2!$A$9:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$B$11</c:f>
+              <c:f>Sheet2!$B$9:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>21.597999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.343</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.042999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.4469999999999992</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.423</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.2230000000000008</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.1920000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.11</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.1790000000000003</c:v>
-                </c:pt>
+                <c:ptCount val="3"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1920,27 +1869,6 @@
                 <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1951,61 +1879,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>73.724000000000004</c:v>
+                  <c:v>85.347999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.803999999999998</c:v>
+                  <c:v>28.364999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.369</c:v>
+                  <c:v>23.452000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.593</c:v>
+                  <c:v>21.56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.585999999999999</c:v>
+                  <c:v>20.533999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.033000000000001</c:v>
+                  <c:v>20.015000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.722999999999999</c:v>
+                  <c:v>19.579000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.594999999999999</c:v>
+                  <c:v>19.459</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.439</c:v>
+                  <c:v>19.387</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.268999999999998</c:v>
+                  <c:v>19.239000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.113</c:v>
+                  <c:v>19.222999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.119</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19.087</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>19.079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>19.201000000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>19.053000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19.055</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>19.149000000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19.079000000000001</c:v>
+                  <c:v>19.268000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,159 +1948,97 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet2!$E$3:$E$51</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>k</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -2202,151 +2047,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>425.69099999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>330.79399999999998</c:v>
+                  <c:v>87.13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87.114999999999995</c:v>
+                  <c:v>67.478999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.373999999999995</c:v>
+                  <c:v>60.908999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60.316000000000003</c:v>
+                  <c:v>57.137</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57.271000000000001</c:v>
+                  <c:v>55.398000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.219000000000001</c:v>
+                  <c:v>54.082999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54.002000000000002</c:v>
+                  <c:v>52.863</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53.067</c:v>
+                  <c:v>52.009</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.466000000000001</c:v>
+                  <c:v>51.343000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.585999999999999</c:v>
+                  <c:v>51.411999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51.206000000000003</c:v>
+                  <c:v>50.685000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50.674999999999997</c:v>
+                  <c:v>50.247</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50.390999999999998</c:v>
+                  <c:v>50.475000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50.195</c:v>
+                  <c:v>50.279000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50.04</c:v>
+                  <c:v>49.686999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>50.152000000000001</c:v>
+                  <c:v>49.825000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>49.92</c:v>
+                  <c:v>49.368000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50.029000000000003</c:v>
+                  <c:v>50.161000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49.686</c:v>
+                  <c:v>49.887</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49.902999999999999</c:v>
+                  <c:v>49.026000000000003</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49.55</c:v>
+                  <c:v>49.786000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>49.17</c:v>
+                  <c:v>49.621000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>49.215000000000003</c:v>
+                  <c:v>49.02</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>49.034999999999997</c:v>
+                  <c:v>48.896000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49.113</c:v>
+                  <c:v>49.277999999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>49.337000000000003</c:v>
+                  <c:v>48.723999999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>48.613999999999997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>49.36</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>49.029000000000003</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>49.283999999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>49.578000000000003</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>49.127000000000002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>49.268000000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>49.173000000000002</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>49.066000000000003</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>49.073999999999998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>49.235999999999997</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>48.835999999999999</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>49.552</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>48.981000000000002</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>48.838000000000001</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>49.191000000000003</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>49.082000000000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>48.968000000000004</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>49.110999999999997</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>49.298000000000002</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>49.3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49.274000000000001</c:v>
+                  <c:v>49.165999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2361,11 +2143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="352220720"/>
-        <c:axId val="352221840"/>
+        <c:axId val="223546560"/>
+        <c:axId val="223547120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="352220720"/>
+        <c:axId val="223546560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2483,12 +2265,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352221840"/>
+        <c:crossAx val="223547120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="352221840"/>
+        <c:axId val="223547120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2601,7 +2383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="352220720"/>
+        <c:crossAx val="223546560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5198,15 +4980,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1048576"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5217,596 +4999,361 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>21.597999999999999</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="4">
+        <v>22.748000000000001</v>
+      </c>
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>73.724000000000004</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="4">
+        <v>85.347999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>425.69099999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>11.292</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>28.364999999999998</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4">
+        <v>87.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>23.452000000000002</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>67.478999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9.43</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>21.56</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>60.908999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>11.343</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>28.803999999999998</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>330.79399999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>10.042999999999999</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>23.369</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>87.114999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>9.4469999999999992</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>21.593</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>67.373999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B7" s="4">
+        <v>9.3819999999999997</v>
+      </c>
+      <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>9.423</v>
-      </c>
-      <c r="C7">
+      <c r="D7" s="4">
+        <v>20.533999999999999</v>
+      </c>
+      <c r="E7" s="4">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>20.585999999999999</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>60.316000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="F7" s="4">
+        <v>57.137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>9.2230000000000008</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="4">
+        <v>9.1829999999999998</v>
+      </c>
+      <c r="C8" s="4">
         <v>6</v>
       </c>
-      <c r="D8">
-        <v>20.033000000000001</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>57.271000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="D8" s="4">
+        <v>20.015000000000001</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>55.398000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="4">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>9.1920000000000002</v>
-      </c>
-      <c r="C9">
+      <c r="D9" s="4">
+        <v>19.579000000000001</v>
+      </c>
+      <c r="E9" s="4">
         <v>7</v>
       </c>
-      <c r="D9">
-        <v>19.722999999999999</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>55.219000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F9" s="4">
+        <v>54.082999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="4">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>9.11</v>
-      </c>
-      <c r="C10">
+      <c r="D10" s="4">
+        <v>19.459</v>
+      </c>
+      <c r="E10" s="4">
         <v>8</v>
       </c>
-      <c r="D10">
-        <v>19.594999999999999</v>
-      </c>
-      <c r="E10">
-        <v>7</v>
-      </c>
-      <c r="F10">
-        <v>54.002000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="F10" s="4">
+        <v>52.863</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="4">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>9.1790000000000003</v>
-      </c>
-      <c r="C11">
+      <c r="D11" s="4">
+        <v>19.387</v>
+      </c>
+      <c r="E11" s="4">
         <v>9</v>
       </c>
-      <c r="D11">
-        <v>19.439</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>53.067</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12">
+      <c r="F11" s="4">
+        <v>52.009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12">
-        <v>19.268999999999998</v>
-      </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>52.466000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13">
+      <c r="D12" s="4">
+        <v>19.239000000000001</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4">
+        <v>51.343000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="4">
         <v>11</v>
       </c>
-      <c r="D13">
-        <v>19.113</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>51.585999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14">
+      <c r="D13" s="4">
+        <v>19.222999999999999</v>
+      </c>
+      <c r="E13" s="4">
+        <v>11</v>
+      </c>
+      <c r="F13" s="4">
+        <v>51.411999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="4">
         <v>12</v>
       </c>
-      <c r="D14">
-        <v>19.119</v>
-      </c>
-      <c r="E14">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>51.206000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15">
+      <c r="D14" s="4">
+        <v>19.268000000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4">
+        <v>50.685000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="4">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>19.087</v>
-      </c>
-      <c r="E15">
-        <v>12</v>
-      </c>
-      <c r="F15">
-        <v>50.674999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16">
+      <c r="F15" s="4">
+        <v>50.247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="4">
         <v>14</v>
       </c>
-      <c r="D16">
-        <v>19.079999999999998</v>
-      </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
-      <c r="F16">
-        <v>50.390999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17">
+      <c r="F16" s="4">
+        <v>50.475000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="4">
         <v>15</v>
       </c>
-      <c r="D17">
-        <v>19.201000000000001</v>
-      </c>
-      <c r="E17">
-        <v>14</v>
-      </c>
-      <c r="F17">
-        <v>50.195</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18">
+      <c r="F17" s="4">
+        <v>50.279000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="4">
         <v>16</v>
       </c>
-      <c r="D18">
-        <v>19.053000000000001</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
-      <c r="F18">
-        <v>50.04</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19">
+      <c r="F18" s="4">
+        <v>49.686999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="4">
         <v>17</v>
       </c>
-      <c r="D19">
-        <v>19.055</v>
-      </c>
-      <c r="E19">
-        <v>16</v>
-      </c>
-      <c r="F19">
-        <v>50.152000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20">
+      <c r="F19" s="4">
+        <v>49.825000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="4">
         <v>18</v>
       </c>
-      <c r="D20">
-        <v>19.149000000000001</v>
-      </c>
-      <c r="E20">
-        <v>17</v>
-      </c>
-      <c r="F20">
-        <v>49.92</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21">
+      <c r="F20" s="4">
+        <v>49.368000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="4">
         <v>19</v>
       </c>
-      <c r="D21">
-        <v>19.079000000000001</v>
-      </c>
-      <c r="E21">
-        <v>18</v>
-      </c>
-      <c r="F21">
-        <v>50.029000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <v>19</v>
-      </c>
-      <c r="F22">
-        <v>49.686</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E23">
+      <c r="F21" s="4">
+        <v>50.161000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="4">
         <v>20</v>
       </c>
-      <c r="F23">
-        <v>49.902999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E24">
+      <c r="F22" s="4">
+        <v>49.887</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="4">
         <v>21</v>
       </c>
-      <c r="F24">
-        <v>49.55</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E25">
+      <c r="F23" s="4">
+        <v>49.026000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="4">
         <v>22</v>
       </c>
-      <c r="F25">
-        <v>49.17</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E26">
+      <c r="F24" s="4">
+        <v>49.786000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="4">
         <v>23</v>
       </c>
-      <c r="F26">
-        <v>49.215000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E27">
+      <c r="F25" s="4">
+        <v>49.621000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="4">
         <v>24</v>
       </c>
-      <c r="F27">
-        <v>49.034999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E28">
+      <c r="F26" s="4">
+        <v>49.02</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="4">
         <v>25</v>
       </c>
-      <c r="F28">
-        <v>49.113</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E29">
+      <c r="F27" s="4">
+        <v>48.896000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="4">
         <v>26</v>
       </c>
-      <c r="F29">
-        <v>49.337000000000003</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E30">
+      <c r="F28" s="4">
+        <v>49.277999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="4">
         <v>27</v>
       </c>
-      <c r="F30">
-        <v>48.613999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E31">
+      <c r="F29" s="4">
+        <v>48.723999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="4">
         <v>28</v>
       </c>
-      <c r="F31">
-        <v>49.36</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <v>29</v>
-      </c>
-      <c r="F32">
-        <v>49.029000000000003</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <v>30</v>
-      </c>
-      <c r="F33">
-        <v>49.283999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34">
-        <v>31</v>
-      </c>
-      <c r="F34">
-        <v>49.578000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35">
-        <v>32</v>
-      </c>
-      <c r="F35">
-        <v>49.127000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36">
-        <v>33</v>
-      </c>
-      <c r="F36">
-        <v>49.268000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37">
-        <v>34</v>
-      </c>
-      <c r="F37">
-        <v>49.173000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38">
-        <v>35</v>
-      </c>
-      <c r="F38">
-        <v>49.066000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E39">
-        <v>36</v>
-      </c>
-      <c r="F39">
-        <v>49.073999999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E40">
-        <v>37</v>
-      </c>
-      <c r="F40">
-        <v>49.235999999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E41">
-        <v>38</v>
-      </c>
-      <c r="F41">
-        <v>48.835999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E42">
-        <v>39</v>
-      </c>
-      <c r="F42">
-        <v>49.552</v>
-      </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E43">
-        <v>40</v>
-      </c>
-      <c r="F43">
-        <v>48.981000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E44">
-        <v>41</v>
-      </c>
-      <c r="F44">
-        <v>48.838000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E45">
-        <v>42</v>
-      </c>
-      <c r="F45">
-        <v>49.191000000000003</v>
-      </c>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E46">
-        <v>43</v>
-      </c>
-      <c r="F46">
-        <v>49.082000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E47">
-        <v>44</v>
-      </c>
-      <c r="F47">
-        <v>48.968000000000004</v>
-      </c>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E48">
-        <v>45</v>
-      </c>
-      <c r="F48">
-        <v>49.110999999999997</v>
-      </c>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49">
-        <v>46</v>
-      </c>
-      <c r="F49">
-        <v>49.298000000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E50">
-        <v>47</v>
-      </c>
-      <c r="F50">
-        <v>49.3</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51">
-        <v>48</v>
-      </c>
-      <c r="F51">
-        <v>49.274000000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E52">
-        <v>49</v>
-      </c>
-      <c r="F52">
-        <v>49.078000000000003</v>
+      <c r="F30" s="4">
+        <v>49.165999999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
got nice  color for terrain. Working on implementing a texture
</commit_message>
<xml_diff>
--- a/cs351/proj4/deliverables/charts.xlsx
+++ b/cs351/proj4/deliverables/charts.xlsx
@@ -187,6 +187,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -260,154 +261,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.14000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0.26</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0.32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0.34</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0.36</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0.38</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0.46</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.66</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.72</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,157 +420,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>11.023999999999999</c:v>
+                  <c:v>11.042</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.081</c:v>
+                  <c:v>11.048</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.147</c:v>
+                  <c:v>11.048999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.055</c:v>
+                  <c:v>11.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.218999999999999</c:v>
+                  <c:v>11.132</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.132999999999999</c:v>
+                  <c:v>11.042</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.227</c:v>
+                  <c:v>11.167999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.262</c:v>
+                  <c:v>11.103</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.44</c:v>
+                  <c:v>11.157</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.419</c:v>
+                  <c:v>11.305</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.297000000000001</c:v>
+                  <c:v>11.164</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.315</c:v>
+                  <c:v>11.159000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.505000000000001</c:v>
+                  <c:v>11.23</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>11.183999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.342000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.282999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.265000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.263999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11.435</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.398</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.35</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.397</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.481</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.385999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.378</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.425000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.542999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.555</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>11.486000000000001</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>11.439</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11.563000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11.61</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11.629</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11.667999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11.63</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11.657999999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11.67</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.775</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>11.63</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>11.638</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="30">
+                  <c:v>11.507999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.545999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.499000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.518000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.493</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11.555</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.526999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.558999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.561999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>11.647</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>11.597</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>11.826000000000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>11.792999999999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>11.647</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>11.738</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>11.87</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>11.811</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>11.81</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>11.775</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>11.769</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>11.788</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>11.85</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>11.773999999999999</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>11.766999999999999</c:v>
-                </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.691000000000001</c:v>
+                  <c:v>11.532</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.753</c:v>
+                  <c:v>11.49</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.709</c:v>
+                  <c:v>11.670999999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11.781000000000001</c:v>
+                  <c:v>11.561</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>11.682</c:v>
+                  <c:v>11.612</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>11.781000000000001</c:v>
+                  <c:v>11.672000000000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11.651999999999999</c:v>
+                  <c:v>11.715</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11.673999999999999</c:v>
+                  <c:v>11.613</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>11.612</c:v>
+                  <c:v>11.641999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11.576000000000001</c:v>
+                  <c:v>11.685</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>11.723000000000001</c:v>
+                  <c:v>11.771000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -614,154 +615,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.14000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0.26</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0.32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0.34</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0.36</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0.38</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0.46</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.66</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.72</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -773,157 +774,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>35.027000000000001</c:v>
+                  <c:v>34.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.884</c:v>
+                  <c:v>34.293999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.966999999999999</c:v>
+                  <c:v>34.027999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.484000000000002</c:v>
+                  <c:v>33.051000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.033999999999999</c:v>
+                  <c:v>33.155999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.024000000000001</c:v>
+                  <c:v>32.761000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.992999999999999</c:v>
+                  <c:v>32.633000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.216999999999999</c:v>
+                  <c:v>32.301000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.925000000000001</c:v>
+                  <c:v>31.844000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.948</c:v>
+                  <c:v>31.867999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.173999999999999</c:v>
+                  <c:v>31.27</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.132999999999999</c:v>
+                  <c:v>31.210999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.167999999999999</c:v>
+                  <c:v>31.123000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.852</c:v>
+                  <c:v>30.352</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28.984000000000002</c:v>
+                  <c:v>30.428999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.571999999999999</c:v>
+                  <c:v>30.364000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.372</c:v>
+                  <c:v>30.045999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28.009</c:v>
+                  <c:v>29.898</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28.152000000000001</c:v>
+                  <c:v>29.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28.109000000000002</c:v>
+                  <c:v>29.329000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>28.097000000000001</c:v>
+                  <c:v>29.370999999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>28.311</c:v>
+                  <c:v>29.175000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27.85</c:v>
+                  <c:v>29.045000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>27.978000000000002</c:v>
+                  <c:v>29.218</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>27.693999999999999</c:v>
+                  <c:v>28.969000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>27.588000000000001</c:v>
+                  <c:v>29.004999999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27.696999999999999</c:v>
+                  <c:v>28.867000000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.824000000000002</c:v>
+                  <c:v>28.89</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>27.968</c:v>
+                  <c:v>28.488</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>27.46</c:v>
+                  <c:v>28.414999999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>28.081</c:v>
+                  <c:v>28.641999999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>27.370999999999999</c:v>
+                  <c:v>28.530999999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>27.734000000000002</c:v>
+                  <c:v>28.637</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27.652000000000001</c:v>
+                  <c:v>28.268000000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>27.696000000000002</c:v>
+                  <c:v>28.344000000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>27.731000000000002</c:v>
+                  <c:v>27.998000000000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>27.306000000000001</c:v>
+                  <c:v>28.259</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>27.669</c:v>
+                  <c:v>28.152999999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>27.824000000000002</c:v>
+                  <c:v>27.748999999999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>27.827999999999999</c:v>
+                  <c:v>27.902999999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>27.565000000000001</c:v>
+                  <c:v>27.989000000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>27.888000000000002</c:v>
+                  <c:v>27.756</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27.943000000000001</c:v>
+                  <c:v>27.956</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>28.085999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>27.815000000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>27.651</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>27.997</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>27.667000000000002</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>27.602</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>27.885000000000002</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>27.773</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>27.978999999999999</c:v>
-                </c:pt>
                 <c:pt idx="48">
-                  <c:v>27.408000000000001</c:v>
+                  <c:v>27.702000000000002</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>27.523</c:v>
+                  <c:v>27.917999999999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>27.707999999999998</c:v>
+                  <c:v>28.271999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,154 +969,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0.14000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="23">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="25">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>0.26</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="29">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>0.3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="31">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0.32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="33">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0.34</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="35">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0.36</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="37">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>0.38</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="39">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="41">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>0.42</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="43">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>0.44</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0.46</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="47">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="49">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.52</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.54</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.56000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.62</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.64</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.66</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.72</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.88</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.92</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.98</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,157 +1128,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>185.32599999999999</c:v>
+                  <c:v>183.99199999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>162.09399999999999</c:v>
+                  <c:v>171.96600000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>141.04599999999999</c:v>
+                  <c:v>159.05500000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.16999999999999</c:v>
+                  <c:v>148.971</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118.53100000000001</c:v>
+                  <c:v>141.73699999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109.922</c:v>
+                  <c:v>132.648</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>103.96599999999999</c:v>
+                  <c:v>126.80200000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100.321</c:v>
+                  <c:v>121.80500000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>95.796000000000006</c:v>
+                  <c:v>117.544</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>93.557000000000002</c:v>
+                  <c:v>113.108</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>91.503</c:v>
+                  <c:v>110.56</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.263000000000005</c:v>
+                  <c:v>106.343</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>87.594999999999999</c:v>
+                  <c:v>104.21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85.674000000000007</c:v>
+                  <c:v>102.032</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84.986999999999995</c:v>
+                  <c:v>99.772000000000006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83.921999999999997</c:v>
+                  <c:v>97.971000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>83.108000000000004</c:v>
+                  <c:v>96.454999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>82.064999999999998</c:v>
+                  <c:v>94.438000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>81.444000000000003</c:v>
+                  <c:v>93.122</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>80.661000000000001</c:v>
+                  <c:v>92.85</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>79.659000000000006</c:v>
+                  <c:v>91.51</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>78.814999999999998</c:v>
+                  <c:v>89.653999999999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>78.427000000000007</c:v>
+                  <c:v>89.683999999999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>79.364000000000004</c:v>
+                  <c:v>87.656000000000006</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>78.858000000000004</c:v>
+                  <c:v>87.268000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>78.355999999999995</c:v>
+                  <c:v>86.093999999999994</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>78.325999999999993</c:v>
+                  <c:v>85.215000000000003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>77.863</c:v>
+                  <c:v>84.662999999999997</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>78.090999999999994</c:v>
+                  <c:v>85.132999999999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>77.489999999999995</c:v>
+                  <c:v>84.254000000000005</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>77.942999999999998</c:v>
+                  <c:v>83.278000000000006</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>77.662000000000006</c:v>
+                  <c:v>83.12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>77.8</c:v>
+                  <c:v>82.13</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>77.909000000000006</c:v>
+                  <c:v>82.738</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>76.930000000000007</c:v>
+                  <c:v>82.512</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>78.653999999999996</c:v>
+                  <c:v>81.944999999999993</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>77.403000000000006</c:v>
+                  <c:v>81.182000000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>76.989000000000004</c:v>
+                  <c:v>80.168999999999997</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>77.144999999999996</c:v>
+                  <c:v>80.471999999999994</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>77.665999999999997</c:v>
+                  <c:v>80.200999999999993</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>77.034000000000006</c:v>
+                  <c:v>80.216999999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>76.989999999999995</c:v>
+                  <c:v>79.433000000000007</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>77.03</c:v>
+                  <c:v>79.209999999999994</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>76.661000000000001</c:v>
+                  <c:v>79.643000000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>76.591999999999999</c:v>
+                  <c:v>79.783000000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>77.012</c:v>
+                  <c:v>78.623000000000005</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>77.509</c:v>
+                  <c:v>79.39</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>77.474999999999994</c:v>
+                  <c:v>78.296000000000006</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>77.293000000000006</c:v>
+                  <c:v>78.353999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>77.266000000000005</c:v>
+                  <c:v>78.003</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>77.564999999999998</c:v>
+                  <c:v>78.275000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1347,6 +1348,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1464,6 +1466,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1544,6 +1547,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1781,19 +1785,55 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$9:$A$11</c:f>
+              <c:f>Sheet2!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$9:$B$11</c:f>
+              <c:f>Sheet2!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>22.748000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3819999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1829999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1829,10 +1869,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$C$3:$C$21</c:f>
+              <c:f>Sheet2!$C$3:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1874,10 +1914,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$3:$D$21</c:f>
+              <c:f>Sheet2!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>85.347999999999999</c:v>
                 </c:pt>
@@ -1949,10 +1989,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$E$3:$E$51</c:f>
+              <c:f>Sheet2!$E$3:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2042,10 +2082,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$F$3:$F$51</c:f>
+              <c:f>Sheet2!$F$3:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>425.69099999999997</c:v>
                 </c:pt>
@@ -3909,10 +3949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,1019 +3996,1419 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>11.023999999999999</v>
+        <v>11.042</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>35.027000000000001</v>
+        <v>34.96</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>185.32599999999999</v>
+        <v>183.99199999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="B4" s="2">
-        <v>11.081</v>
+        <v>11.048</v>
       </c>
       <c r="C4" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D4" s="2">
-        <v>33.884</v>
+        <v>34.293999999999997</v>
       </c>
       <c r="E4" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F4" s="2">
-        <v>162.09399999999999</v>
+        <v>171.96600000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="B5" s="2">
-        <v>11.147</v>
+        <v>11.048999999999999</v>
       </c>
       <c r="C5" s="2">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="D5" s="2">
-        <v>32.966999999999999</v>
+        <v>34.027999999999999</v>
       </c>
       <c r="E5" s="2">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F5" s="2">
-        <v>141.04599999999999</v>
+        <v>159.05500000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="B6" s="2">
-        <v>11.055</v>
+        <v>11.03</v>
       </c>
       <c r="C6" s="2">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="D6" s="2">
-        <v>32.484000000000002</v>
+        <v>33.051000000000002</v>
       </c>
       <c r="E6" s="2">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F6" s="2">
-        <v>128.16999999999999</v>
+        <v>148.971</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="B7" s="2">
-        <v>11.218999999999999</v>
+        <v>11.132</v>
       </c>
       <c r="C7" s="2">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="D7" s="2">
-        <v>32.033999999999999</v>
+        <v>33.155999999999999</v>
       </c>
       <c r="E7" s="2">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="F7" s="2">
-        <v>118.53100000000001</v>
+        <v>141.73699999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="B8" s="2">
-        <v>11.132999999999999</v>
+        <v>11.042</v>
       </c>
       <c r="C8" s="2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D8" s="2">
-        <v>31.024000000000001</v>
+        <v>32.761000000000003</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F8" s="2">
-        <v>109.922</v>
+        <v>132.648</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="B9" s="2">
-        <v>11.227</v>
+        <v>11.167999999999999</v>
       </c>
       <c r="C9" s="2">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="D9" s="2">
-        <v>30.992999999999999</v>
+        <v>32.633000000000003</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="F9" s="2">
-        <v>103.96599999999999</v>
+        <v>126.80200000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="B10" s="2">
-        <v>11.262</v>
+        <v>11.103</v>
       </c>
       <c r="C10" s="2">
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>30.216999999999999</v>
+        <v>32.301000000000002</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>100.321</v>
+        <v>121.80500000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="B11" s="2">
-        <v>11.44</v>
+        <v>11.157</v>
       </c>
       <c r="C11" s="2">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="D11" s="2">
-        <v>29.925000000000001</v>
+        <v>31.844000000000001</v>
       </c>
       <c r="E11" s="2">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="F11" s="2">
-        <v>95.796000000000006</v>
+        <v>117.544</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="B12" s="2">
-        <v>11.419</v>
+        <v>11.305</v>
       </c>
       <c r="C12" s="2">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="D12" s="2">
-        <v>29.948</v>
+        <v>31.867999999999999</v>
       </c>
       <c r="E12" s="2">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F12" s="2">
-        <v>93.557000000000002</v>
+        <v>113.108</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="B13" s="2">
-        <v>11.297000000000001</v>
+        <v>11.164</v>
       </c>
       <c r="C13" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D13" s="2">
-        <v>29.173999999999999</v>
+        <v>31.27</v>
       </c>
       <c r="E13" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F13" s="2">
-        <v>91.503</v>
+        <v>110.56</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="B14" s="2">
-        <v>11.315</v>
+        <v>11.159000000000001</v>
       </c>
       <c r="C14" s="2">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="D14" s="2">
-        <v>29.132999999999999</v>
+        <v>31.210999999999999</v>
       </c>
       <c r="E14" s="2">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="F14" s="2">
-        <v>89.263000000000005</v>
+        <v>106.343</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="B15" s="2">
-        <v>11.505000000000001</v>
+        <v>11.23</v>
       </c>
       <c r="C15" s="2">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="D15" s="2">
-        <v>29.167999999999999</v>
+        <v>31.123000000000001</v>
       </c>
       <c r="E15" s="2">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="F15" s="2">
-        <v>87.594999999999999</v>
+        <v>104.21</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="B16" s="2">
-        <v>11.486000000000001</v>
+        <v>11.183999999999999</v>
       </c>
       <c r="C16" s="2">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="D16" s="2">
-        <v>28.852</v>
+        <v>30.352</v>
       </c>
       <c r="E16" s="2">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="F16" s="2">
-        <v>85.674000000000007</v>
+        <v>102.032</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="B17" s="2">
-        <v>11.439</v>
+        <v>11.19</v>
       </c>
       <c r="C17" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D17" s="2">
-        <v>28.984000000000002</v>
+        <v>30.428999999999998</v>
       </c>
       <c r="E17" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F17" s="2">
-        <v>84.986999999999995</v>
+        <v>99.772000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="B18" s="2">
-        <v>11.563000000000001</v>
+        <v>11.342000000000001</v>
       </c>
       <c r="C18" s="2">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="D18" s="2">
-        <v>28.571999999999999</v>
+        <v>30.364000000000001</v>
       </c>
       <c r="E18" s="2">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="F18" s="2">
-        <v>83.921999999999997</v>
+        <v>97.971000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
-        <v>0.32</v>
+        <v>0.16</v>
       </c>
       <c r="B19" s="2">
-        <v>11.61</v>
+        <v>11.282999999999999</v>
       </c>
       <c r="C19" s="2">
-        <v>0.32</v>
+        <v>0.16</v>
       </c>
       <c r="D19" s="2">
-        <v>28.372</v>
+        <v>30.045999999999999</v>
       </c>
       <c r="E19" s="2">
-        <v>0.32</v>
+        <v>0.16</v>
       </c>
       <c r="F19" s="2">
-        <v>83.108000000000004</v>
+        <v>96.454999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
-        <v>0.34</v>
+        <v>0.17</v>
       </c>
       <c r="B20" s="2">
-        <v>11.629</v>
+        <v>11.265000000000001</v>
       </c>
       <c r="C20" s="2">
-        <v>0.34</v>
+        <v>0.17</v>
       </c>
       <c r="D20" s="2">
-        <v>28.009</v>
+        <v>29.898</v>
       </c>
       <c r="E20" s="2">
-        <v>0.34</v>
+        <v>0.17</v>
       </c>
       <c r="F20" s="2">
-        <v>82.064999999999998</v>
+        <v>94.438000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="B21" s="2">
-        <v>11.667999999999999</v>
+        <v>11.263999999999999</v>
       </c>
       <c r="C21" s="2">
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="D21" s="2">
-        <v>28.152000000000001</v>
+        <v>29.75</v>
       </c>
       <c r="E21" s="2">
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
       <c r="F21" s="2">
-        <v>81.444000000000003</v>
+        <v>93.122</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <v>0.38</v>
+        <v>0.19</v>
       </c>
       <c r="B22" s="2">
-        <v>11.63</v>
+        <v>11.435</v>
       </c>
       <c r="C22" s="2">
-        <v>0.38</v>
+        <v>0.19</v>
       </c>
       <c r="D22" s="2">
-        <v>28.109000000000002</v>
+        <v>29.329000000000001</v>
       </c>
       <c r="E22" s="2">
-        <v>0.38</v>
+        <v>0.19</v>
       </c>
       <c r="F22" s="2">
-        <v>80.661000000000001</v>
+        <v>92.85</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="B23" s="2">
-        <v>11.657999999999999</v>
+        <v>11.398</v>
       </c>
       <c r="C23" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="2">
-        <v>28.097000000000001</v>
+        <v>29.370999999999999</v>
       </c>
       <c r="E23" s="2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F23" s="2">
-        <v>79.659000000000006</v>
+        <v>91.51</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>0.42</v>
+        <v>0.21</v>
       </c>
       <c r="B24" s="2">
-        <v>11.67</v>
+        <v>11.35</v>
       </c>
       <c r="C24" s="2">
-        <v>0.42</v>
+        <v>0.21</v>
       </c>
       <c r="D24" s="2">
-        <v>28.311</v>
+        <v>29.175000000000001</v>
       </c>
       <c r="E24" s="2">
-        <v>0.42</v>
+        <v>0.21</v>
       </c>
       <c r="F24" s="2">
-        <v>78.814999999999998</v>
+        <v>89.653999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="B25" s="2">
-        <v>11.775</v>
+        <v>11.397</v>
       </c>
       <c r="C25" s="2">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="D25" s="2">
-        <v>27.85</v>
+        <v>29.045000000000002</v>
       </c>
       <c r="E25" s="2">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="F25" s="2">
-        <v>78.427000000000007</v>
+        <v>89.683999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>0.46</v>
+        <v>0.23</v>
       </c>
       <c r="B26" s="2">
-        <v>11.63</v>
+        <v>11.481</v>
       </c>
       <c r="C26" s="2">
-        <v>0.46</v>
+        <v>0.23</v>
       </c>
       <c r="D26" s="2">
-        <v>27.978000000000002</v>
+        <v>29.218</v>
       </c>
       <c r="E26" s="2">
-        <v>0.46</v>
+        <v>0.23</v>
       </c>
       <c r="F26" s="2">
-        <v>79.364000000000004</v>
+        <v>87.656000000000006</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>0.48</v>
+        <v>0.24</v>
       </c>
       <c r="B27" s="2">
-        <v>11.638</v>
+        <v>11.385999999999999</v>
       </c>
       <c r="C27" s="2">
-        <v>0.48</v>
+        <v>0.24</v>
       </c>
       <c r="D27" s="2">
-        <v>27.693999999999999</v>
+        <v>28.969000000000001</v>
       </c>
       <c r="E27" s="2">
-        <v>0.48</v>
+        <v>0.24</v>
       </c>
       <c r="F27" s="2">
-        <v>78.858000000000004</v>
+        <v>87.268000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="B28" s="2">
-        <v>11.647</v>
+        <v>11.378</v>
       </c>
       <c r="C28" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D28" s="2">
-        <v>27.588000000000001</v>
+        <v>29.004999999999999</v>
       </c>
       <c r="E28" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F28" s="2">
-        <v>78.355999999999995</v>
+        <v>86.093999999999994</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
-        <v>0.52</v>
+        <v>0.26</v>
       </c>
       <c r="B29" s="2">
-        <v>11.597</v>
+        <v>11.425000000000001</v>
       </c>
       <c r="C29" s="2">
-        <v>0.52</v>
+        <v>0.26</v>
       </c>
       <c r="D29" s="2">
-        <v>27.696999999999999</v>
+        <v>28.867000000000001</v>
       </c>
       <c r="E29" s="2">
-        <v>0.52</v>
+        <v>0.26</v>
       </c>
       <c r="F29" s="2">
-        <v>78.325999999999993</v>
+        <v>85.215000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
-        <v>0.54</v>
+        <v>0.27</v>
       </c>
       <c r="B30" s="2">
-        <v>11.826000000000001</v>
+        <v>11.542999999999999</v>
       </c>
       <c r="C30" s="2">
-        <v>0.54</v>
+        <v>0.27</v>
       </c>
       <c r="D30" s="2">
-        <v>27.824000000000002</v>
+        <v>28.89</v>
       </c>
       <c r="E30" s="2">
-        <v>0.54</v>
+        <v>0.27</v>
       </c>
       <c r="F30" s="2">
-        <v>77.863</v>
+        <v>84.662999999999997</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="B31" s="2">
-        <v>11.792999999999999</v>
+        <v>11.555</v>
       </c>
       <c r="C31" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D31" s="2">
-        <v>27.968</v>
+        <v>28.488</v>
       </c>
       <c r="E31" s="2">
-        <v>0.56000000000000005</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F31" s="2">
-        <v>78.090999999999994</v>
+        <v>85.132999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="B32" s="2">
-        <v>11.647</v>
+        <v>11.486000000000001</v>
       </c>
       <c r="C32" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D32" s="2">
-        <v>27.46</v>
+        <v>28.414999999999999</v>
       </c>
       <c r="E32" s="2">
-        <v>0.57999999999999996</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F32" s="2">
-        <v>77.489999999999995</v>
+        <v>84.254000000000005</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="B33" s="2">
-        <v>11.738</v>
+        <v>11.507999999999999</v>
       </c>
       <c r="C33" s="2">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D33" s="2">
-        <v>28.081</v>
+        <v>28.641999999999999</v>
       </c>
       <c r="E33" s="2">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F33" s="2">
-        <v>77.942999999999998</v>
+        <v>83.278000000000006</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
-        <v>0.62</v>
+        <v>0.31</v>
       </c>
       <c r="B34" s="2">
-        <v>11.87</v>
+        <v>11.545999999999999</v>
       </c>
       <c r="C34" s="2">
-        <v>0.62</v>
+        <v>0.31</v>
       </c>
       <c r="D34" s="2">
-        <v>27.370999999999999</v>
+        <v>28.530999999999999</v>
       </c>
       <c r="E34" s="2">
-        <v>0.62</v>
+        <v>0.31</v>
       </c>
       <c r="F34" s="2">
-        <v>77.662000000000006</v>
+        <v>83.12</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
-        <v>0.64</v>
+        <v>0.32</v>
       </c>
       <c r="B35" s="2">
-        <v>11.811</v>
+        <v>11.499000000000001</v>
       </c>
       <c r="C35" s="2">
-        <v>0.64</v>
+        <v>0.32</v>
       </c>
       <c r="D35" s="2">
-        <v>27.734000000000002</v>
+        <v>28.637</v>
       </c>
       <c r="E35" s="2">
-        <v>0.64</v>
+        <v>0.32</v>
       </c>
       <c r="F35" s="2">
-        <v>77.8</v>
+        <v>82.13</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
-        <v>0.66</v>
+        <v>0.33</v>
       </c>
       <c r="B36" s="2">
-        <v>11.81</v>
+        <v>11.518000000000001</v>
       </c>
       <c r="C36" s="2">
-        <v>0.66</v>
+        <v>0.33</v>
       </c>
       <c r="D36" s="2">
-        <v>27.652000000000001</v>
+        <v>28.268000000000001</v>
       </c>
       <c r="E36" s="2">
-        <v>0.66</v>
+        <v>0.33</v>
       </c>
       <c r="F36" s="2">
-        <v>77.909000000000006</v>
+        <v>82.738</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
-        <v>0.68</v>
+        <v>0.34</v>
       </c>
       <c r="B37" s="2">
-        <v>11.775</v>
+        <v>11.493</v>
       </c>
       <c r="C37" s="2">
-        <v>0.68</v>
+        <v>0.34</v>
       </c>
       <c r="D37" s="2">
-        <v>27.696000000000002</v>
+        <v>28.344000000000001</v>
       </c>
       <c r="E37" s="2">
-        <v>0.68</v>
+        <v>0.34</v>
       </c>
       <c r="F37" s="2">
-        <v>76.930000000000007</v>
+        <v>82.512</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="B38" s="2">
-        <v>11.769</v>
+        <v>11.555</v>
       </c>
       <c r="C38" s="2">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="D38" s="2">
-        <v>27.731000000000002</v>
+        <v>27.998000000000001</v>
       </c>
       <c r="E38" s="2">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
       <c r="F38" s="2">
-        <v>78.653999999999996</v>
+        <v>81.944999999999993</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
       <c r="B39" s="2">
-        <v>11.788</v>
+        <v>11.526999999999999</v>
       </c>
       <c r="C39" s="2">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
       <c r="D39" s="2">
-        <v>27.306000000000001</v>
+        <v>28.259</v>
       </c>
       <c r="E39" s="2">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
       <c r="F39" s="2">
-        <v>77.403000000000006</v>
+        <v>81.182000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
-        <v>0.74</v>
+        <v>0.37</v>
       </c>
       <c r="B40" s="2">
-        <v>11.85</v>
+        <v>11.558999999999999</v>
       </c>
       <c r="C40" s="2">
-        <v>0.74</v>
+        <v>0.37</v>
       </c>
       <c r="D40" s="2">
-        <v>27.669</v>
+        <v>28.152999999999999</v>
       </c>
       <c r="E40" s="2">
-        <v>0.74</v>
+        <v>0.37</v>
       </c>
       <c r="F40" s="2">
-        <v>76.989000000000004</v>
+        <v>80.168999999999997</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
-        <v>0.76</v>
+        <v>0.38</v>
       </c>
       <c r="B41" s="2">
-        <v>11.773999999999999</v>
+        <v>11.561999999999999</v>
       </c>
       <c r="C41" s="2">
-        <v>0.76</v>
+        <v>0.38</v>
       </c>
       <c r="D41" s="2">
-        <v>27.824000000000002</v>
+        <v>27.748999999999999</v>
       </c>
       <c r="E41" s="2">
-        <v>0.76</v>
+        <v>0.38</v>
       </c>
       <c r="F41" s="2">
-        <v>77.144999999999996</v>
+        <v>80.471999999999994</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
-        <v>0.78</v>
+        <v>0.39</v>
       </c>
       <c r="B42" s="2">
-        <v>11.766999999999999</v>
+        <v>11.647</v>
       </c>
       <c r="C42" s="2">
-        <v>0.78</v>
+        <v>0.39</v>
       </c>
       <c r="D42" s="2">
-        <v>27.827999999999999</v>
+        <v>27.902999999999999</v>
       </c>
       <c r="E42" s="2">
-        <v>0.78</v>
+        <v>0.39</v>
       </c>
       <c r="F42" s="2">
-        <v>77.665999999999997</v>
+        <v>80.200999999999993</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="B43" s="2">
-        <v>11.691000000000001</v>
+        <v>11.532</v>
       </c>
       <c r="C43" s="2">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D43" s="2">
-        <v>27.565000000000001</v>
+        <v>27.989000000000001</v>
       </c>
       <c r="E43" s="2">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F43" s="2">
-        <v>77.034000000000006</v>
+        <v>80.216999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
-        <v>0.82</v>
+        <v>0.41</v>
       </c>
       <c r="B44" s="2">
-        <v>11.753</v>
+        <v>11.49</v>
       </c>
       <c r="C44" s="2">
-        <v>0.82</v>
+        <v>0.41</v>
       </c>
       <c r="D44" s="2">
-        <v>27.888000000000002</v>
+        <v>27.756</v>
       </c>
       <c r="E44" s="2">
-        <v>0.82</v>
+        <v>0.41</v>
       </c>
       <c r="F44" s="2">
-        <v>76.989999999999995</v>
+        <v>79.433000000000007</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
-        <v>0.84</v>
+        <v>0.42</v>
       </c>
       <c r="B45" s="2">
-        <v>11.709</v>
+        <v>11.670999999999999</v>
       </c>
       <c r="C45" s="2">
-        <v>0.84</v>
+        <v>0.42</v>
       </c>
       <c r="D45" s="2">
-        <v>27.943000000000001</v>
+        <v>27.956</v>
       </c>
       <c r="E45" s="2">
-        <v>0.84</v>
+        <v>0.42</v>
       </c>
       <c r="F45" s="2">
-        <v>77.03</v>
+        <v>79.209999999999994</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
-        <v>0.86</v>
+        <v>0.43</v>
       </c>
       <c r="B46" s="2">
-        <v>11.781000000000001</v>
+        <v>11.561</v>
       </c>
       <c r="C46" s="2">
-        <v>0.86</v>
+        <v>0.43</v>
       </c>
       <c r="D46" s="2">
-        <v>27.667000000000002</v>
+        <v>28.085999999999999</v>
       </c>
       <c r="E46" s="2">
-        <v>0.86</v>
+        <v>0.43</v>
       </c>
       <c r="F46" s="2">
-        <v>76.661000000000001</v>
+        <v>79.643000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>0.88</v>
+        <v>0.44</v>
       </c>
       <c r="B47" s="2">
-        <v>11.682</v>
+        <v>11.612</v>
       </c>
       <c r="C47" s="2">
-        <v>0.88</v>
+        <v>0.44</v>
       </c>
       <c r="D47" s="2">
-        <v>27.602</v>
+        <v>27.815000000000001</v>
       </c>
       <c r="E47" s="2">
-        <v>0.88</v>
+        <v>0.44</v>
       </c>
       <c r="F47" s="2">
-        <v>76.591999999999999</v>
+        <v>79.783000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="B48" s="2">
-        <v>11.781000000000001</v>
+        <v>11.672000000000001</v>
       </c>
       <c r="C48" s="2">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="D48" s="2">
-        <v>27.885000000000002</v>
+        <v>27.651</v>
       </c>
       <c r="E48" s="2">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
       <c r="F48" s="2">
-        <v>77.012</v>
+        <v>78.623000000000005</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>0.92</v>
+        <v>0.46</v>
       </c>
       <c r="B49" s="2">
-        <v>11.651999999999999</v>
+        <v>11.715</v>
       </c>
       <c r="C49" s="2">
-        <v>0.92</v>
+        <v>0.46</v>
       </c>
       <c r="D49" s="2">
-        <v>27.773</v>
+        <v>27.997</v>
       </c>
       <c r="E49" s="2">
-        <v>0.92</v>
+        <v>0.46</v>
       </c>
       <c r="F49" s="2">
-        <v>77.509</v>
+        <v>79.39</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>0.94</v>
+        <v>0.47</v>
       </c>
       <c r="B50" s="2">
-        <v>11.673999999999999</v>
+        <v>11.613</v>
       </c>
       <c r="C50" s="2">
-        <v>0.94</v>
+        <v>0.47</v>
       </c>
       <c r="D50" s="2">
-        <v>27.978999999999999</v>
+        <v>27.667000000000002</v>
       </c>
       <c r="E50" s="2">
-        <v>0.94</v>
+        <v>0.47</v>
       </c>
       <c r="F50" s="2">
-        <v>77.474999999999994</v>
+        <v>78.296000000000006</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="B51" s="2">
-        <v>11.612</v>
+        <v>11.641999999999999</v>
       </c>
       <c r="C51" s="2">
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="D51" s="2">
-        <v>27.408000000000001</v>
+        <v>27.702000000000002</v>
       </c>
       <c r="E51" s="2">
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="F51" s="2">
-        <v>77.293000000000006</v>
+        <v>78.353999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
-        <v>0.98</v>
+        <v>0.49</v>
       </c>
       <c r="B52" s="2">
-        <v>11.576000000000001</v>
+        <v>11.685</v>
       </c>
       <c r="C52" s="2">
-        <v>0.98</v>
+        <v>0.49</v>
       </c>
       <c r="D52" s="2">
-        <v>27.523</v>
+        <v>27.917999999999999</v>
       </c>
       <c r="E52" s="2">
-        <v>0.98</v>
+        <v>0.49</v>
       </c>
       <c r="F52" s="2">
-        <v>77.266000000000005</v>
+        <v>78.003</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B53" s="2">
-        <v>11.723000000000001</v>
+        <v>11.771000000000001</v>
       </c>
       <c r="C53" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D53" s="2">
-        <v>27.707999999999998</v>
+        <v>28.271999999999998</v>
       </c>
       <c r="E53" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F53" s="2">
-        <v>77.564999999999998</v>
+        <v>78.275000000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.51</v>
+      </c>
+      <c r="B54">
+        <v>11.77</v>
+      </c>
+      <c r="C54">
+        <v>0.51</v>
+      </c>
+      <c r="D54">
+        <v>27.834</v>
+      </c>
+      <c r="E54">
+        <v>0.51</v>
+      </c>
+      <c r="F54">
+        <v>78.23</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0.52</v>
+      </c>
+      <c r="B55">
+        <v>11.69</v>
+      </c>
+      <c r="C55">
+        <v>0.52</v>
+      </c>
+      <c r="D55">
+        <v>27.802</v>
+      </c>
+      <c r="E55">
+        <v>0.52</v>
+      </c>
+      <c r="F55">
+        <v>78.893000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.53</v>
+      </c>
+      <c r="B56">
+        <v>11.644</v>
+      </c>
+      <c r="C56">
+        <v>0.53</v>
+      </c>
+      <c r="D56">
+        <v>27.829000000000001</v>
+      </c>
+      <c r="E56">
+        <v>0.53</v>
+      </c>
+      <c r="F56">
+        <v>78.498000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.54</v>
+      </c>
+      <c r="B57">
+        <v>11.693</v>
+      </c>
+      <c r="C57">
+        <v>0.54</v>
+      </c>
+      <c r="D57">
+        <v>27.956</v>
+      </c>
+      <c r="E57">
+        <v>0.54</v>
+      </c>
+      <c r="F57">
+        <v>77.738</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B58">
+        <v>11.614000000000001</v>
+      </c>
+      <c r="C58">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D58">
+        <v>28.013999999999999</v>
+      </c>
+      <c r="E58">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F58">
+        <v>77.096000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B59">
+        <v>11.635999999999999</v>
+      </c>
+      <c r="C59">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D59">
+        <v>27.952999999999999</v>
+      </c>
+      <c r="E59">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F59">
+        <v>77.521000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="B60">
+        <v>11.776</v>
+      </c>
+      <c r="C60">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D60">
+        <v>27.885999999999999</v>
+      </c>
+      <c r="E60">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F60">
+        <v>78.340999999999994</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B61">
+        <v>11.722</v>
+      </c>
+      <c r="C61">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D61">
+        <v>27.783000000000001</v>
+      </c>
+      <c r="E61">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F61">
+        <v>77.540999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.59</v>
+      </c>
+      <c r="B62">
+        <v>11.69</v>
+      </c>
+      <c r="C62">
+        <v>0.59</v>
+      </c>
+      <c r="D62">
+        <v>28.097000000000001</v>
+      </c>
+      <c r="E62">
+        <v>0.59</v>
+      </c>
+      <c r="F62">
+        <v>77.367000000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0.6</v>
+      </c>
+      <c r="B63">
+        <v>11.726000000000001</v>
+      </c>
+      <c r="C63">
+        <v>0.6</v>
+      </c>
+      <c r="D63">
+        <v>28.052</v>
+      </c>
+      <c r="E63">
+        <v>0.6</v>
+      </c>
+      <c r="F63">
+        <v>77.183999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>0.61</v>
+      </c>
+      <c r="B64">
+        <v>11.728</v>
+      </c>
+      <c r="C64">
+        <v>0.61</v>
+      </c>
+      <c r="D64">
+        <v>27.78</v>
+      </c>
+      <c r="E64">
+        <v>0.61</v>
+      </c>
+      <c r="F64">
+        <v>76.927000000000007</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.62</v>
+      </c>
+      <c r="B65">
+        <v>11.813000000000001</v>
+      </c>
+      <c r="C65">
+        <v>0.62</v>
+      </c>
+      <c r="D65">
+        <v>27.948</v>
+      </c>
+      <c r="E65">
+        <v>0.62</v>
+      </c>
+      <c r="F65">
+        <v>77.509</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.63</v>
+      </c>
+      <c r="B66">
+        <v>11.79</v>
+      </c>
+      <c r="C66">
+        <v>0.63</v>
+      </c>
+      <c r="D66">
+        <v>27.425000000000001</v>
+      </c>
+      <c r="E66">
+        <v>0.63</v>
+      </c>
+      <c r="F66">
+        <v>77.734999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.64</v>
+      </c>
+      <c r="B67">
+        <v>11.657</v>
+      </c>
+      <c r="C67">
+        <v>0.64</v>
+      </c>
+      <c r="D67">
+        <v>27.858000000000001</v>
+      </c>
+      <c r="E67">
+        <v>0.64</v>
+      </c>
+      <c r="F67">
+        <v>77.352000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.65</v>
+      </c>
+      <c r="B68">
+        <v>11.682</v>
+      </c>
+      <c r="C68">
+        <v>0.65</v>
+      </c>
+      <c r="D68">
+        <v>27.672000000000001</v>
+      </c>
+      <c r="E68">
+        <v>0.65</v>
+      </c>
+      <c r="F68">
+        <v>77.114999999999995</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.66</v>
+      </c>
+      <c r="B69">
+        <v>11.692</v>
+      </c>
+      <c r="C69">
+        <v>0.66</v>
+      </c>
+      <c r="D69">
+        <v>27.629000000000001</v>
+      </c>
+      <c r="E69">
+        <v>0.66</v>
+      </c>
+      <c r="F69">
+        <v>77.912999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.67</v>
+      </c>
+      <c r="B70">
+        <v>11.683999999999999</v>
+      </c>
+      <c r="C70">
+        <v>0.67</v>
+      </c>
+      <c r="D70">
+        <v>27.611999999999998</v>
+      </c>
+      <c r="E70">
+        <v>0.67</v>
+      </c>
+      <c r="F70">
+        <v>77.81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0.68</v>
+      </c>
+      <c r="B71">
+        <v>11.71</v>
+      </c>
+      <c r="C71">
+        <v>0.68</v>
+      </c>
+      <c r="D71">
+        <v>27.858000000000001</v>
+      </c>
+      <c r="E71">
+        <v>0.68</v>
+      </c>
+      <c r="F71">
+        <v>77.171000000000006</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0.69</v>
+      </c>
+      <c r="B72">
+        <v>11.888999999999999</v>
+      </c>
+      <c r="C72">
+        <v>0.69</v>
+      </c>
+      <c r="D72">
+        <v>27.946999999999999</v>
+      </c>
+      <c r="E72">
+        <v>0.69</v>
+      </c>
+      <c r="F72">
+        <v>77.566999999999993</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>0.7</v>
+      </c>
+      <c r="B73">
+        <v>11.757999999999999</v>
+      </c>
+      <c r="C73">
+        <v>0.7</v>
+      </c>
+      <c r="D73">
+        <v>27.696000000000002</v>
+      </c>
+      <c r="E73">
+        <v>0.7</v>
+      </c>
+      <c r="F73">
+        <v>77.367999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -4983,7 +5423,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cs711 : checkpoint 7 attempt
</commit_message>
<xml_diff>
--- a/cs351/proj4/deliverables/charts.xlsx
+++ b/cs351/proj4/deliverables/charts.xlsx
@@ -420,157 +420,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>11.042</c:v>
+                  <c:v>22.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.048</c:v>
+                  <c:v>22.029</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.048999999999999</c:v>
+                  <c:v>22.030999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.03</c:v>
+                  <c:v>22.193999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.132</c:v>
+                  <c:v>22.263000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.042</c:v>
+                  <c:v>22.123999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.167999999999999</c:v>
+                  <c:v>22.219000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.103</c:v>
+                  <c:v>22.337</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.157</c:v>
+                  <c:v>22.242000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.305</c:v>
+                  <c:v>22.623999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.164</c:v>
+                  <c:v>22.388000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.159000000000001</c:v>
+                  <c:v>22.257000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.23</c:v>
+                  <c:v>22.472999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.183999999999999</c:v>
+                  <c:v>22.356000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.19</c:v>
+                  <c:v>22.649000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.342000000000001</c:v>
+                  <c:v>22.577999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.282999999999999</c:v>
+                  <c:v>22.53</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.265000000000001</c:v>
+                  <c:v>22.710999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.263999999999999</c:v>
+                  <c:v>22.765000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.435</c:v>
+                  <c:v>22.780999999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.398</c:v>
+                  <c:v>22.611999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.35</c:v>
+                  <c:v>22.908000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.397</c:v>
+                  <c:v>22.855</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11.481</c:v>
+                  <c:v>22.885999999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11.385999999999999</c:v>
+                  <c:v>22.795999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11.378</c:v>
+                  <c:v>22.943999999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.425000000000001</c:v>
+                  <c:v>22.91</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11.542999999999999</c:v>
+                  <c:v>23.109000000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11.555</c:v>
+                  <c:v>23.030999999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11.486000000000001</c:v>
+                  <c:v>22.821000000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>11.507999999999999</c:v>
+                  <c:v>22.995000000000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.545999999999999</c:v>
+                  <c:v>23.108000000000001</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11.499000000000001</c:v>
+                  <c:v>23.215</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.518000000000001</c:v>
+                  <c:v>22.818999999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.493</c:v>
+                  <c:v>23.102</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.555</c:v>
+                  <c:v>23.102</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.526999999999999</c:v>
+                  <c:v>23.172000000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.558999999999999</c:v>
+                  <c:v>23.120999999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11.561999999999999</c:v>
+                  <c:v>22.992000000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.647</c:v>
+                  <c:v>23.207999999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.532</c:v>
+                  <c:v>23.123000000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.49</c:v>
+                  <c:v>23.248000000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.670999999999999</c:v>
+                  <c:v>23.446000000000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11.561</c:v>
+                  <c:v>23.245000000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>11.612</c:v>
+                  <c:v>23.407</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>11.672000000000001</c:v>
+                  <c:v>23.256</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11.715</c:v>
+                  <c:v>23.103000000000002</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11.613</c:v>
+                  <c:v>23.373000000000001</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>11.641999999999999</c:v>
+                  <c:v>23.253</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11.685</c:v>
+                  <c:v>23.14</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>11.771000000000001</c:v>
+                  <c:v>23.283000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -774,157 +774,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>34.96</c:v>
+                  <c:v>68.426000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34.293999999999997</c:v>
+                  <c:v>68.790999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.027999999999999</c:v>
+                  <c:v>67.667000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.051000000000002</c:v>
+                  <c:v>67.102000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33.155999999999999</c:v>
+                  <c:v>66.418000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.761000000000003</c:v>
+                  <c:v>64.861999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.633000000000003</c:v>
+                  <c:v>64.891000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.301000000000002</c:v>
+                  <c:v>63.832999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.844000000000001</c:v>
+                  <c:v>63.948</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.867999999999999</c:v>
+                  <c:v>63.052999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.27</c:v>
+                  <c:v>63.137</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31.210999999999999</c:v>
+                  <c:v>62.942999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31.123000000000001</c:v>
+                  <c:v>61.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30.352</c:v>
+                  <c:v>61.276000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>30.428999999999998</c:v>
+                  <c:v>60.674999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30.364000000000001</c:v>
+                  <c:v>60.454999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.045999999999999</c:v>
+                  <c:v>59.963999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.898</c:v>
+                  <c:v>59.417000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.75</c:v>
+                  <c:v>59.350999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.329000000000001</c:v>
+                  <c:v>59.167999999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.370999999999999</c:v>
+                  <c:v>58.884</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>29.175000000000001</c:v>
+                  <c:v>58.537999999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>29.045000000000002</c:v>
+                  <c:v>58.843000000000004</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>29.218</c:v>
+                  <c:v>58.197000000000003</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28.969000000000001</c:v>
+                  <c:v>58.722999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29.004999999999999</c:v>
+                  <c:v>57.584000000000003</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>28.867000000000001</c:v>
+                  <c:v>57.503</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28.89</c:v>
+                  <c:v>57.442</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.488</c:v>
+                  <c:v>57.377000000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>28.414999999999999</c:v>
+                  <c:v>56.921999999999997</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>28.641999999999999</c:v>
+                  <c:v>56.765999999999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>28.530999999999999</c:v>
+                  <c:v>56.606000000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>28.637</c:v>
+                  <c:v>56.621000000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>28.268000000000001</c:v>
+                  <c:v>56.713999999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>28.344000000000001</c:v>
+                  <c:v>56.62</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>27.998000000000001</c:v>
+                  <c:v>56.445999999999998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>28.259</c:v>
+                  <c:v>56.61</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>28.152999999999999</c:v>
+                  <c:v>56.33</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>27.748999999999999</c:v>
+                  <c:v>55.978000000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>27.902999999999999</c:v>
+                  <c:v>56.008000000000003</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>27.989000000000001</c:v>
+                  <c:v>55.981999999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>27.756</c:v>
+                  <c:v>56.485999999999997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27.956</c:v>
+                  <c:v>55.965000000000003</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>28.085999999999999</c:v>
+                  <c:v>56.116999999999997</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>27.815000000000001</c:v>
+                  <c:v>55.98</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>27.651</c:v>
+                  <c:v>55.722999999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>27.997</c:v>
+                  <c:v>55.098999999999997</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>27.667000000000002</c:v>
+                  <c:v>55.545999999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>27.702000000000002</c:v>
+                  <c:v>55.295999999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>27.917999999999999</c:v>
+                  <c:v>55.283000000000001</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>28.271999999999998</c:v>
+                  <c:v>56.192999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,157 +1128,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>183.99199999999999</c:v>
+                  <c:v>376.34300000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.96600000000001</c:v>
+                  <c:v>344.565</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159.05500000000001</c:v>
+                  <c:v>317.858</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>148.971</c:v>
+                  <c:v>299.36500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141.73699999999999</c:v>
+                  <c:v>282.81599999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>132.648</c:v>
+                  <c:v>267.745</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>126.80200000000001</c:v>
+                  <c:v>252.11099999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>121.80500000000001</c:v>
+                  <c:v>245.06800000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>117.544</c:v>
+                  <c:v>236.745</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>113.108</c:v>
+                  <c:v>227.13399999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>110.56</c:v>
+                  <c:v>220.405</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>106.343</c:v>
+                  <c:v>213.76900000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.21</c:v>
+                  <c:v>208.36600000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>102.032</c:v>
+                  <c:v>203.917</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>99.772000000000006</c:v>
+                  <c:v>200.166</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>97.971000000000004</c:v>
+                  <c:v>195.77799999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>96.454999999999998</c:v>
+                  <c:v>192.94300000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>94.438000000000002</c:v>
+                  <c:v>190.251</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>93.122</c:v>
+                  <c:v>187.22399999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>92.85</c:v>
+                  <c:v>184.03899999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>91.51</c:v>
+                  <c:v>182.602</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>89.653999999999996</c:v>
+                  <c:v>178.572</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>89.683999999999997</c:v>
+                  <c:v>178.05</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>87.656000000000006</c:v>
+                  <c:v>175.328</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>87.268000000000001</c:v>
+                  <c:v>173.63900000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>86.093999999999994</c:v>
+                  <c:v>173.35400000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>85.215000000000003</c:v>
+                  <c:v>169.86500000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>84.662999999999997</c:v>
+                  <c:v>169.631</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>85.132999999999996</c:v>
+                  <c:v>168.643</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>84.254000000000005</c:v>
+                  <c:v>166.73699999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>83.278000000000006</c:v>
+                  <c:v>167.85300000000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>83.12</c:v>
+                  <c:v>166.928</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>82.13</c:v>
+                  <c:v>163.792</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>82.738</c:v>
+                  <c:v>162.32300000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>82.512</c:v>
+                  <c:v>165.00299999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>81.944999999999993</c:v>
+                  <c:v>162.922</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>81.182000000000002</c:v>
+                  <c:v>163.16800000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>80.168999999999997</c:v>
+                  <c:v>161.65299999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>80.471999999999994</c:v>
+                  <c:v>160.934</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>80.200999999999993</c:v>
+                  <c:v>161.11000000000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>80.216999999999999</c:v>
+                  <c:v>159.49100000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>79.433000000000007</c:v>
+                  <c:v>159.25800000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>79.209999999999994</c:v>
+                  <c:v>157.91499999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>79.643000000000001</c:v>
+                  <c:v>158.76</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>79.783000000000001</c:v>
+                  <c:v>159.71899999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>78.623000000000005</c:v>
+                  <c:v>157.364</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>79.39</c:v>
+                  <c:v>157.334</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>78.296000000000006</c:v>
+                  <c:v>157.40700000000001</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>78.353999999999999</c:v>
+                  <c:v>156.41399999999999</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>78.003</c:v>
+                  <c:v>155.578</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>78.275000000000006</c:v>
+                  <c:v>155.53100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,11 +1293,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="221453472"/>
-        <c:axId val="221454592"/>
+        <c:axId val="196999968"/>
+        <c:axId val="197000528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="221453472"/>
+        <c:axId val="196999968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,12 +1415,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221454592"/>
+        <c:crossAx val="197000528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="221454592"/>
+        <c:axId val="197000528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,7 +1533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221453472"/>
+        <c:crossAx val="196999968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1817,22 +1817,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>22.748000000000001</c:v>
+                  <c:v>43.454000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.292</c:v>
+                  <c:v>22.338999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.050000000000001</c:v>
+                  <c:v>19.768000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.43</c:v>
+                  <c:v>18.603999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3819999999999997</c:v>
+                  <c:v>18.466999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.1829999999999998</c:v>
+                  <c:v>18.213000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,40 +1919,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>85.347999999999999</c:v>
+                  <c:v>177.053</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.364999999999998</c:v>
+                  <c:v>62.835999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.452000000000002</c:v>
+                  <c:v>48.167999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.56</c:v>
+                  <c:v>43.064999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.533999999999999</c:v>
+                  <c:v>41.371000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.015000000000001</c:v>
+                  <c:v>39.871000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.579000000000001</c:v>
+                  <c:v>39.209000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.459</c:v>
+                  <c:v>38.743000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.387</c:v>
+                  <c:v>38.393999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.239000000000001</c:v>
+                  <c:v>38.079000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.222999999999999</c:v>
+                  <c:v>38.073</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.268000000000001</c:v>
+                  <c:v>38.195</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2087,88 +2087,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>425.69099999999997</c:v>
+                  <c:v>1046.684</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.13</c:v>
+                  <c:v>223.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.478999999999999</c:v>
+                  <c:v>158.041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.908999999999999</c:v>
+                  <c:v>135.417</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.137</c:v>
+                  <c:v>124.072</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55.398000000000003</c:v>
+                  <c:v>116.199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54.082999999999998</c:v>
+                  <c:v>111.149</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52.863</c:v>
+                  <c:v>107.60299999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.009</c:v>
+                  <c:v>106.495</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51.343000000000004</c:v>
+                  <c:v>104.836</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>51.411999999999999</c:v>
+                  <c:v>102.304</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>50.685000000000002</c:v>
+                  <c:v>101.749</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>50.247</c:v>
+                  <c:v>101.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>50.475000000000001</c:v>
+                  <c:v>100.89</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50.279000000000003</c:v>
+                  <c:v>99.393000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49.686999999999998</c:v>
+                  <c:v>99.561000000000007</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>49.825000000000003</c:v>
+                  <c:v>99.171000000000006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>49.368000000000002</c:v>
+                  <c:v>99.74</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50.161000000000001</c:v>
+                  <c:v>100.456</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49.887</c:v>
+                  <c:v>98.298000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49.026000000000003</c:v>
+                  <c:v>97.942999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49.786000000000001</c:v>
+                  <c:v>98.296000000000006</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>49.621000000000002</c:v>
+                  <c:v>97.86</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>49.02</c:v>
+                  <c:v>98.747</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>48.896000000000001</c:v>
+                  <c:v>98.882000000000005</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49.277999999999999</c:v>
+                  <c:v>98.867999999999995</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>48.723999999999997</c:v>
+                  <c:v>98.418000000000006</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>49.165999999999997</c:v>
+                  <c:v>98.569000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2183,11 +2183,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223546560"/>
-        <c:axId val="223547120"/>
+        <c:axId val="199930368"/>
+        <c:axId val="199930928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223546560"/>
+        <c:axId val="199930368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,12 +2305,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223547120"/>
+        <c:crossAx val="199930928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223547120"/>
+        <c:axId val="199930928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2423,7 +2423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223546560"/>
+        <c:crossAx val="199930368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3951,8 +3951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection sqref="A1:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,19 +3996,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>11.042</v>
+        <v>22.15</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>34.96</v>
+        <v>68.426000000000002</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>183.99199999999999</v>
+        <v>376.34300000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4016,19 +4016,19 @@
         <v>0.01</v>
       </c>
       <c r="B4" s="2">
-        <v>11.048</v>
+        <v>22.029</v>
       </c>
       <c r="C4" s="2">
         <v>0.01</v>
       </c>
       <c r="D4" s="2">
-        <v>34.293999999999997</v>
+        <v>68.790999999999997</v>
       </c>
       <c r="E4" s="2">
         <v>0.01</v>
       </c>
       <c r="F4" s="2">
-        <v>171.96600000000001</v>
+        <v>344.565</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4036,19 +4036,19 @@
         <v>0.02</v>
       </c>
       <c r="B5" s="2">
-        <v>11.048999999999999</v>
+        <v>22.030999999999999</v>
       </c>
       <c r="C5" s="2">
         <v>0.02</v>
       </c>
       <c r="D5" s="2">
-        <v>34.027999999999999</v>
+        <v>67.667000000000002</v>
       </c>
       <c r="E5" s="2">
         <v>0.02</v>
       </c>
       <c r="F5" s="2">
-        <v>159.05500000000001</v>
+        <v>317.858</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4056,19 +4056,19 @@
         <v>0.03</v>
       </c>
       <c r="B6" s="2">
-        <v>11.03</v>
+        <v>22.193999999999999</v>
       </c>
       <c r="C6" s="2">
         <v>0.03</v>
       </c>
       <c r="D6" s="2">
-        <v>33.051000000000002</v>
+        <v>67.102000000000004</v>
       </c>
       <c r="E6" s="2">
         <v>0.03</v>
       </c>
       <c r="F6" s="2">
-        <v>148.971</v>
+        <v>299.36500000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4076,19 +4076,19 @@
         <v>0.04</v>
       </c>
       <c r="B7" s="2">
-        <v>11.132</v>
+        <v>22.263000000000002</v>
       </c>
       <c r="C7" s="2">
         <v>0.04</v>
       </c>
       <c r="D7" s="2">
-        <v>33.155999999999999</v>
+        <v>66.418000000000006</v>
       </c>
       <c r="E7" s="2">
         <v>0.04</v>
       </c>
       <c r="F7" s="2">
-        <v>141.73699999999999</v>
+        <v>282.81599999999997</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4096,19 +4096,19 @@
         <v>0.05</v>
       </c>
       <c r="B8" s="2">
-        <v>11.042</v>
+        <v>22.123999999999999</v>
       </c>
       <c r="C8" s="2">
         <v>0.05</v>
       </c>
       <c r="D8" s="2">
-        <v>32.761000000000003</v>
+        <v>64.861999999999995</v>
       </c>
       <c r="E8" s="2">
         <v>0.05</v>
       </c>
       <c r="F8" s="2">
-        <v>132.648</v>
+        <v>267.745</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4116,19 +4116,19 @@
         <v>0.06</v>
       </c>
       <c r="B9" s="2">
-        <v>11.167999999999999</v>
+        <v>22.219000000000001</v>
       </c>
       <c r="C9" s="2">
         <v>0.06</v>
       </c>
       <c r="D9" s="2">
-        <v>32.633000000000003</v>
+        <v>64.891000000000005</v>
       </c>
       <c r="E9" s="2">
         <v>0.06</v>
       </c>
       <c r="F9" s="2">
-        <v>126.80200000000001</v>
+        <v>252.11099999999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4136,19 +4136,19 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B10" s="2">
-        <v>11.103</v>
+        <v>22.337</v>
       </c>
       <c r="C10" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>32.301000000000002</v>
+        <v>63.832999999999998</v>
       </c>
       <c r="E10" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F10" s="2">
-        <v>121.80500000000001</v>
+        <v>245.06800000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4156,19 +4156,19 @@
         <v>0.08</v>
       </c>
       <c r="B11" s="2">
-        <v>11.157</v>
+        <v>22.242000000000001</v>
       </c>
       <c r="C11" s="2">
         <v>0.08</v>
       </c>
       <c r="D11" s="2">
-        <v>31.844000000000001</v>
+        <v>63.948</v>
       </c>
       <c r="E11" s="2">
         <v>0.08</v>
       </c>
       <c r="F11" s="2">
-        <v>117.544</v>
+        <v>236.745</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4176,19 +4176,19 @@
         <v>0.09</v>
       </c>
       <c r="B12" s="2">
-        <v>11.305</v>
+        <v>22.623999999999999</v>
       </c>
       <c r="C12" s="2">
         <v>0.09</v>
       </c>
       <c r="D12" s="2">
-        <v>31.867999999999999</v>
+        <v>63.052999999999997</v>
       </c>
       <c r="E12" s="2">
         <v>0.09</v>
       </c>
       <c r="F12" s="2">
-        <v>113.108</v>
+        <v>227.13399999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4196,19 +4196,19 @@
         <v>0.1</v>
       </c>
       <c r="B13" s="2">
-        <v>11.164</v>
+        <v>22.388000000000002</v>
       </c>
       <c r="C13" s="2">
         <v>0.1</v>
       </c>
       <c r="D13" s="2">
-        <v>31.27</v>
+        <v>63.137</v>
       </c>
       <c r="E13" s="2">
         <v>0.1</v>
       </c>
       <c r="F13" s="2">
-        <v>110.56</v>
+        <v>220.405</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4216,19 +4216,19 @@
         <v>0.11</v>
       </c>
       <c r="B14" s="2">
-        <v>11.159000000000001</v>
+        <v>22.257000000000001</v>
       </c>
       <c r="C14" s="2">
         <v>0.11</v>
       </c>
       <c r="D14" s="2">
-        <v>31.210999999999999</v>
+        <v>62.942999999999998</v>
       </c>
       <c r="E14" s="2">
         <v>0.11</v>
       </c>
       <c r="F14" s="2">
-        <v>106.343</v>
+        <v>213.76900000000001</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4236,19 +4236,19 @@
         <v>0.12</v>
       </c>
       <c r="B15" s="2">
-        <v>11.23</v>
+        <v>22.472999999999999</v>
       </c>
       <c r="C15" s="2">
         <v>0.12</v>
       </c>
       <c r="D15" s="2">
-        <v>31.123000000000001</v>
+        <v>61.9</v>
       </c>
       <c r="E15" s="2">
         <v>0.12</v>
       </c>
       <c r="F15" s="2">
-        <v>104.21</v>
+        <v>208.36600000000001</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4256,19 +4256,19 @@
         <v>0.13</v>
       </c>
       <c r="B16" s="2">
-        <v>11.183999999999999</v>
+        <v>22.356000000000002</v>
       </c>
       <c r="C16" s="2">
         <v>0.13</v>
       </c>
       <c r="D16" s="2">
-        <v>30.352</v>
+        <v>61.276000000000003</v>
       </c>
       <c r="E16" s="2">
         <v>0.13</v>
       </c>
       <c r="F16" s="2">
-        <v>102.032</v>
+        <v>203.917</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4276,19 +4276,19 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="B17" s="2">
-        <v>11.19</v>
+        <v>22.649000000000001</v>
       </c>
       <c r="C17" s="2">
         <v>0.14000000000000001</v>
       </c>
       <c r="D17" s="2">
-        <v>30.428999999999998</v>
+        <v>60.674999999999997</v>
       </c>
       <c r="E17" s="2">
         <v>0.14000000000000001</v>
       </c>
       <c r="F17" s="2">
-        <v>99.772000000000006</v>
+        <v>200.166</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4296,19 +4296,19 @@
         <v>0.15</v>
       </c>
       <c r="B18" s="2">
-        <v>11.342000000000001</v>
+        <v>22.577999999999999</v>
       </c>
       <c r="C18" s="2">
         <v>0.15</v>
       </c>
       <c r="D18" s="2">
-        <v>30.364000000000001</v>
+        <v>60.454999999999998</v>
       </c>
       <c r="E18" s="2">
         <v>0.15</v>
       </c>
       <c r="F18" s="2">
-        <v>97.971000000000004</v>
+        <v>195.77799999999999</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4316,19 +4316,19 @@
         <v>0.16</v>
       </c>
       <c r="B19" s="2">
-        <v>11.282999999999999</v>
+        <v>22.53</v>
       </c>
       <c r="C19" s="2">
         <v>0.16</v>
       </c>
       <c r="D19" s="2">
-        <v>30.045999999999999</v>
+        <v>59.963999999999999</v>
       </c>
       <c r="E19" s="2">
         <v>0.16</v>
       </c>
       <c r="F19" s="2">
-        <v>96.454999999999998</v>
+        <v>192.94300000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4336,19 +4336,19 @@
         <v>0.17</v>
       </c>
       <c r="B20" s="2">
-        <v>11.265000000000001</v>
+        <v>22.710999999999999</v>
       </c>
       <c r="C20" s="2">
         <v>0.17</v>
       </c>
       <c r="D20" s="2">
-        <v>29.898</v>
+        <v>59.417000000000002</v>
       </c>
       <c r="E20" s="2">
         <v>0.17</v>
       </c>
       <c r="F20" s="2">
-        <v>94.438000000000002</v>
+        <v>190.251</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4356,19 +4356,19 @@
         <v>0.18</v>
       </c>
       <c r="B21" s="2">
-        <v>11.263999999999999</v>
+        <v>22.765000000000001</v>
       </c>
       <c r="C21" s="2">
         <v>0.18</v>
       </c>
       <c r="D21" s="2">
-        <v>29.75</v>
+        <v>59.350999999999999</v>
       </c>
       <c r="E21" s="2">
         <v>0.18</v>
       </c>
       <c r="F21" s="2">
-        <v>93.122</v>
+        <v>187.22399999999999</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4376,19 +4376,19 @@
         <v>0.19</v>
       </c>
       <c r="B22" s="2">
-        <v>11.435</v>
+        <v>22.780999999999999</v>
       </c>
       <c r="C22" s="2">
         <v>0.19</v>
       </c>
       <c r="D22" s="2">
-        <v>29.329000000000001</v>
+        <v>59.167999999999999</v>
       </c>
       <c r="E22" s="2">
         <v>0.19</v>
       </c>
       <c r="F22" s="2">
-        <v>92.85</v>
+        <v>184.03899999999999</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4396,19 +4396,19 @@
         <v>0.2</v>
       </c>
       <c r="B23" s="2">
-        <v>11.398</v>
+        <v>22.611999999999998</v>
       </c>
       <c r="C23" s="2">
         <v>0.2</v>
       </c>
       <c r="D23" s="2">
-        <v>29.370999999999999</v>
+        <v>58.884</v>
       </c>
       <c r="E23" s="2">
         <v>0.2</v>
       </c>
       <c r="F23" s="2">
-        <v>91.51</v>
+        <v>182.602</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4416,19 +4416,19 @@
         <v>0.21</v>
       </c>
       <c r="B24" s="2">
-        <v>11.35</v>
+        <v>22.908000000000001</v>
       </c>
       <c r="C24" s="2">
         <v>0.21</v>
       </c>
       <c r="D24" s="2">
-        <v>29.175000000000001</v>
+        <v>58.537999999999997</v>
       </c>
       <c r="E24" s="2">
         <v>0.21</v>
       </c>
       <c r="F24" s="2">
-        <v>89.653999999999996</v>
+        <v>178.572</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4436,19 +4436,19 @@
         <v>0.22</v>
       </c>
       <c r="B25" s="2">
-        <v>11.397</v>
+        <v>22.855</v>
       </c>
       <c r="C25" s="2">
         <v>0.22</v>
       </c>
       <c r="D25" s="2">
-        <v>29.045000000000002</v>
+        <v>58.843000000000004</v>
       </c>
       <c r="E25" s="2">
         <v>0.22</v>
       </c>
       <c r="F25" s="2">
-        <v>89.683999999999997</v>
+        <v>178.05</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4456,19 +4456,19 @@
         <v>0.23</v>
       </c>
       <c r="B26" s="2">
-        <v>11.481</v>
+        <v>22.885999999999999</v>
       </c>
       <c r="C26" s="2">
         <v>0.23</v>
       </c>
       <c r="D26" s="2">
-        <v>29.218</v>
+        <v>58.197000000000003</v>
       </c>
       <c r="E26" s="2">
         <v>0.23</v>
       </c>
       <c r="F26" s="2">
-        <v>87.656000000000006</v>
+        <v>175.328</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4476,19 +4476,19 @@
         <v>0.24</v>
       </c>
       <c r="B27" s="2">
-        <v>11.385999999999999</v>
+        <v>22.795999999999999</v>
       </c>
       <c r="C27" s="2">
         <v>0.24</v>
       </c>
       <c r="D27" s="2">
-        <v>28.969000000000001</v>
+        <v>58.722999999999999</v>
       </c>
       <c r="E27" s="2">
         <v>0.24</v>
       </c>
       <c r="F27" s="2">
-        <v>87.268000000000001</v>
+        <v>173.63900000000001</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4496,19 +4496,19 @@
         <v>0.25</v>
       </c>
       <c r="B28" s="2">
-        <v>11.378</v>
+        <v>22.943999999999999</v>
       </c>
       <c r="C28" s="2">
         <v>0.25</v>
       </c>
       <c r="D28" s="2">
-        <v>29.004999999999999</v>
+        <v>57.584000000000003</v>
       </c>
       <c r="E28" s="2">
         <v>0.25</v>
       </c>
       <c r="F28" s="2">
-        <v>86.093999999999994</v>
+        <v>173.35400000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4516,19 +4516,19 @@
         <v>0.26</v>
       </c>
       <c r="B29" s="2">
-        <v>11.425000000000001</v>
+        <v>22.91</v>
       </c>
       <c r="C29" s="2">
         <v>0.26</v>
       </c>
       <c r="D29" s="2">
-        <v>28.867000000000001</v>
+        <v>57.503</v>
       </c>
       <c r="E29" s="2">
         <v>0.26</v>
       </c>
       <c r="F29" s="2">
-        <v>85.215000000000003</v>
+        <v>169.86500000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4536,19 +4536,19 @@
         <v>0.27</v>
       </c>
       <c r="B30" s="2">
-        <v>11.542999999999999</v>
+        <v>23.109000000000002</v>
       </c>
       <c r="C30" s="2">
         <v>0.27</v>
       </c>
       <c r="D30" s="2">
-        <v>28.89</v>
+        <v>57.442</v>
       </c>
       <c r="E30" s="2">
         <v>0.27</v>
       </c>
       <c r="F30" s="2">
-        <v>84.662999999999997</v>
+        <v>169.631</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4556,19 +4556,19 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="B31" s="2">
-        <v>11.555</v>
+        <v>23.030999999999999</v>
       </c>
       <c r="C31" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="D31" s="2">
-        <v>28.488</v>
+        <v>57.377000000000002</v>
       </c>
       <c r="E31" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="F31" s="2">
-        <v>85.132999999999996</v>
+        <v>168.643</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4576,19 +4576,19 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="B32" s="2">
-        <v>11.486000000000001</v>
+        <v>22.821000000000002</v>
       </c>
       <c r="C32" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="D32" s="2">
-        <v>28.414999999999999</v>
+        <v>56.921999999999997</v>
       </c>
       <c r="E32" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="F32" s="2">
-        <v>84.254000000000005</v>
+        <v>166.73699999999999</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4596,19 +4596,19 @@
         <v>0.3</v>
       </c>
       <c r="B33" s="2">
-        <v>11.507999999999999</v>
+        <v>22.995000000000001</v>
       </c>
       <c r="C33" s="2">
         <v>0.3</v>
       </c>
       <c r="D33" s="2">
-        <v>28.641999999999999</v>
+        <v>56.765999999999998</v>
       </c>
       <c r="E33" s="2">
         <v>0.3</v>
       </c>
       <c r="F33" s="2">
-        <v>83.278000000000006</v>
+        <v>167.85300000000001</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4616,19 +4616,19 @@
         <v>0.31</v>
       </c>
       <c r="B34" s="2">
-        <v>11.545999999999999</v>
+        <v>23.108000000000001</v>
       </c>
       <c r="C34" s="2">
         <v>0.31</v>
       </c>
       <c r="D34" s="2">
-        <v>28.530999999999999</v>
+        <v>56.606000000000002</v>
       </c>
       <c r="E34" s="2">
         <v>0.31</v>
       </c>
       <c r="F34" s="2">
-        <v>83.12</v>
+        <v>166.928</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4636,19 +4636,19 @@
         <v>0.32</v>
       </c>
       <c r="B35" s="2">
-        <v>11.499000000000001</v>
+        <v>23.215</v>
       </c>
       <c r="C35" s="2">
         <v>0.32</v>
       </c>
       <c r="D35" s="2">
-        <v>28.637</v>
+        <v>56.621000000000002</v>
       </c>
       <c r="E35" s="2">
         <v>0.32</v>
       </c>
       <c r="F35" s="2">
-        <v>82.13</v>
+        <v>163.792</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4656,19 +4656,19 @@
         <v>0.33</v>
       </c>
       <c r="B36" s="2">
-        <v>11.518000000000001</v>
+        <v>22.818999999999999</v>
       </c>
       <c r="C36" s="2">
         <v>0.33</v>
       </c>
       <c r="D36" s="2">
-        <v>28.268000000000001</v>
+        <v>56.713999999999999</v>
       </c>
       <c r="E36" s="2">
         <v>0.33</v>
       </c>
       <c r="F36" s="2">
-        <v>82.738</v>
+        <v>162.32300000000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4676,19 +4676,19 @@
         <v>0.34</v>
       </c>
       <c r="B37" s="2">
-        <v>11.493</v>
+        <v>23.102</v>
       </c>
       <c r="C37" s="2">
         <v>0.34</v>
       </c>
       <c r="D37" s="2">
-        <v>28.344000000000001</v>
+        <v>56.62</v>
       </c>
       <c r="E37" s="2">
         <v>0.34</v>
       </c>
       <c r="F37" s="2">
-        <v>82.512</v>
+        <v>165.00299999999999</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4696,19 +4696,19 @@
         <v>0.35</v>
       </c>
       <c r="B38" s="2">
-        <v>11.555</v>
+        <v>23.102</v>
       </c>
       <c r="C38" s="2">
         <v>0.35</v>
       </c>
       <c r="D38" s="2">
-        <v>27.998000000000001</v>
+        <v>56.445999999999998</v>
       </c>
       <c r="E38" s="2">
         <v>0.35</v>
       </c>
       <c r="F38" s="2">
-        <v>81.944999999999993</v>
+        <v>162.922</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4716,19 +4716,19 @@
         <v>0.36</v>
       </c>
       <c r="B39" s="2">
-        <v>11.526999999999999</v>
+        <v>23.172000000000001</v>
       </c>
       <c r="C39" s="2">
         <v>0.36</v>
       </c>
       <c r="D39" s="2">
-        <v>28.259</v>
+        <v>56.61</v>
       </c>
       <c r="E39" s="2">
         <v>0.36</v>
       </c>
       <c r="F39" s="2">
-        <v>81.182000000000002</v>
+        <v>163.16800000000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4736,19 +4736,19 @@
         <v>0.37</v>
       </c>
       <c r="B40" s="2">
-        <v>11.558999999999999</v>
+        <v>23.120999999999999</v>
       </c>
       <c r="C40" s="2">
         <v>0.37</v>
       </c>
       <c r="D40" s="2">
-        <v>28.152999999999999</v>
+        <v>56.33</v>
       </c>
       <c r="E40" s="2">
         <v>0.37</v>
       </c>
       <c r="F40" s="2">
-        <v>80.168999999999997</v>
+        <v>161.65299999999999</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4756,19 +4756,19 @@
         <v>0.38</v>
       </c>
       <c r="B41" s="2">
-        <v>11.561999999999999</v>
+        <v>22.992000000000001</v>
       </c>
       <c r="C41" s="2">
         <v>0.38</v>
       </c>
       <c r="D41" s="2">
-        <v>27.748999999999999</v>
+        <v>55.978000000000002</v>
       </c>
       <c r="E41" s="2">
         <v>0.38</v>
       </c>
       <c r="F41" s="2">
-        <v>80.471999999999994</v>
+        <v>160.934</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4776,19 +4776,19 @@
         <v>0.39</v>
       </c>
       <c r="B42" s="2">
-        <v>11.647</v>
+        <v>23.207999999999998</v>
       </c>
       <c r="C42" s="2">
         <v>0.39</v>
       </c>
       <c r="D42" s="2">
-        <v>27.902999999999999</v>
+        <v>56.008000000000003</v>
       </c>
       <c r="E42" s="2">
         <v>0.39</v>
       </c>
       <c r="F42" s="2">
-        <v>80.200999999999993</v>
+        <v>161.11000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4796,19 +4796,19 @@
         <v>0.4</v>
       </c>
       <c r="B43" s="2">
-        <v>11.532</v>
+        <v>23.123000000000001</v>
       </c>
       <c r="C43" s="2">
         <v>0.4</v>
       </c>
       <c r="D43" s="2">
-        <v>27.989000000000001</v>
+        <v>55.981999999999999</v>
       </c>
       <c r="E43" s="2">
         <v>0.4</v>
       </c>
       <c r="F43" s="2">
-        <v>80.216999999999999</v>
+        <v>159.49100000000001</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4816,19 +4816,19 @@
         <v>0.41</v>
       </c>
       <c r="B44" s="2">
-        <v>11.49</v>
+        <v>23.248000000000001</v>
       </c>
       <c r="C44" s="2">
         <v>0.41</v>
       </c>
       <c r="D44" s="2">
-        <v>27.756</v>
+        <v>56.485999999999997</v>
       </c>
       <c r="E44" s="2">
         <v>0.41</v>
       </c>
       <c r="F44" s="2">
-        <v>79.433000000000007</v>
+        <v>159.25800000000001</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4836,19 +4836,19 @@
         <v>0.42</v>
       </c>
       <c r="B45" s="2">
-        <v>11.670999999999999</v>
+        <v>23.446000000000002</v>
       </c>
       <c r="C45" s="2">
         <v>0.42</v>
       </c>
       <c r="D45" s="2">
-        <v>27.956</v>
+        <v>55.965000000000003</v>
       </c>
       <c r="E45" s="2">
         <v>0.42</v>
       </c>
       <c r="F45" s="2">
-        <v>79.209999999999994</v>
+        <v>157.91499999999999</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4856,19 +4856,19 @@
         <v>0.43</v>
       </c>
       <c r="B46" s="2">
-        <v>11.561</v>
+        <v>23.245000000000001</v>
       </c>
       <c r="C46" s="2">
         <v>0.43</v>
       </c>
       <c r="D46" s="2">
-        <v>28.085999999999999</v>
+        <v>56.116999999999997</v>
       </c>
       <c r="E46" s="2">
         <v>0.43</v>
       </c>
       <c r="F46" s="2">
-        <v>79.643000000000001</v>
+        <v>158.76</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4876,19 +4876,19 @@
         <v>0.44</v>
       </c>
       <c r="B47" s="2">
-        <v>11.612</v>
+        <v>23.407</v>
       </c>
       <c r="C47" s="2">
         <v>0.44</v>
       </c>
       <c r="D47" s="2">
-        <v>27.815000000000001</v>
+        <v>55.98</v>
       </c>
       <c r="E47" s="2">
         <v>0.44</v>
       </c>
       <c r="F47" s="2">
-        <v>79.783000000000001</v>
+        <v>159.71899999999999</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4896,19 +4896,19 @@
         <v>0.45</v>
       </c>
       <c r="B48" s="2">
-        <v>11.672000000000001</v>
+        <v>23.256</v>
       </c>
       <c r="C48" s="2">
         <v>0.45</v>
       </c>
       <c r="D48" s="2">
-        <v>27.651</v>
+        <v>55.722999999999999</v>
       </c>
       <c r="E48" s="2">
         <v>0.45</v>
       </c>
       <c r="F48" s="2">
-        <v>78.623000000000005</v>
+        <v>157.364</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4916,19 +4916,19 @@
         <v>0.46</v>
       </c>
       <c r="B49" s="2">
-        <v>11.715</v>
+        <v>23.103000000000002</v>
       </c>
       <c r="C49" s="2">
         <v>0.46</v>
       </c>
       <c r="D49" s="2">
-        <v>27.997</v>
+        <v>55.098999999999997</v>
       </c>
       <c r="E49" s="2">
         <v>0.46</v>
       </c>
       <c r="F49" s="2">
-        <v>79.39</v>
+        <v>157.334</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4936,19 +4936,19 @@
         <v>0.47</v>
       </c>
       <c r="B50" s="2">
-        <v>11.613</v>
+        <v>23.373000000000001</v>
       </c>
       <c r="C50" s="2">
         <v>0.47</v>
       </c>
       <c r="D50" s="2">
-        <v>27.667000000000002</v>
+        <v>55.545999999999999</v>
       </c>
       <c r="E50" s="2">
         <v>0.47</v>
       </c>
       <c r="F50" s="2">
-        <v>78.296000000000006</v>
+        <v>157.40700000000001</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4956,19 +4956,19 @@
         <v>0.48</v>
       </c>
       <c r="B51" s="2">
-        <v>11.641999999999999</v>
+        <v>23.253</v>
       </c>
       <c r="C51" s="2">
         <v>0.48</v>
       </c>
       <c r="D51" s="2">
-        <v>27.702000000000002</v>
+        <v>55.295999999999999</v>
       </c>
       <c r="E51" s="2">
         <v>0.48</v>
       </c>
       <c r="F51" s="2">
-        <v>78.353999999999999</v>
+        <v>156.41399999999999</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4976,19 +4976,19 @@
         <v>0.49</v>
       </c>
       <c r="B52" s="2">
-        <v>11.685</v>
+        <v>23.14</v>
       </c>
       <c r="C52" s="2">
         <v>0.49</v>
       </c>
       <c r="D52" s="2">
-        <v>27.917999999999999</v>
+        <v>55.283000000000001</v>
       </c>
       <c r="E52" s="2">
         <v>0.49</v>
       </c>
       <c r="F52" s="2">
-        <v>78.003</v>
+        <v>155.578</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4996,19 +4996,19 @@
         <v>0.5</v>
       </c>
       <c r="B53" s="2">
-        <v>11.771000000000001</v>
+        <v>23.283000000000001</v>
       </c>
       <c r="C53" s="2">
         <v>0.5</v>
       </c>
       <c r="D53" s="2">
-        <v>28.271999999999998</v>
+        <v>56.192999999999998</v>
       </c>
       <c r="E53" s="2">
         <v>0.5</v>
       </c>
       <c r="F53" s="2">
-        <v>78.275000000000006</v>
+        <v>155.53100000000001</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -5016,19 +5016,19 @@
         <v>0.51</v>
       </c>
       <c r="B54">
-        <v>11.77</v>
+        <v>23.390999999999998</v>
       </c>
       <c r="C54">
         <v>0.51</v>
       </c>
       <c r="D54">
-        <v>27.834</v>
+        <v>55.767000000000003</v>
       </c>
       <c r="E54">
         <v>0.51</v>
       </c>
       <c r="F54">
-        <v>78.23</v>
+        <v>156.48400000000001</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -5036,19 +5036,19 @@
         <v>0.52</v>
       </c>
       <c r="B55">
-        <v>11.69</v>
+        <v>23.359000000000002</v>
       </c>
       <c r="C55">
         <v>0.52</v>
       </c>
       <c r="D55">
-        <v>27.802</v>
+        <v>55.259</v>
       </c>
       <c r="E55">
         <v>0.52</v>
       </c>
       <c r="F55">
-        <v>78.893000000000001</v>
+        <v>155.452</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -5056,19 +5056,19 @@
         <v>0.53</v>
       </c>
       <c r="B56">
-        <v>11.644</v>
+        <v>23.587</v>
       </c>
       <c r="C56">
         <v>0.53</v>
       </c>
       <c r="D56">
-        <v>27.829000000000001</v>
+        <v>56.07</v>
       </c>
       <c r="E56">
         <v>0.53</v>
       </c>
       <c r="F56">
-        <v>78.498000000000005</v>
+        <v>155.548</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -5076,19 +5076,19 @@
         <v>0.54</v>
       </c>
       <c r="B57">
-        <v>11.693</v>
+        <v>23.373999999999999</v>
       </c>
       <c r="C57">
         <v>0.54</v>
       </c>
       <c r="D57">
-        <v>27.956</v>
+        <v>55.822000000000003</v>
       </c>
       <c r="E57">
         <v>0.54</v>
       </c>
       <c r="F57">
-        <v>77.738</v>
+        <v>155.56200000000001</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -5096,19 +5096,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B58">
-        <v>11.614000000000001</v>
+        <v>23.36</v>
       </c>
       <c r="C58">
         <v>0.55000000000000004</v>
       </c>
       <c r="D58">
-        <v>28.013999999999999</v>
+        <v>54.753</v>
       </c>
       <c r="E58">
         <v>0.55000000000000004</v>
       </c>
       <c r="F58">
-        <v>77.096000000000004</v>
+        <v>156.41900000000001</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -5116,19 +5116,19 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="B59">
-        <v>11.635999999999999</v>
+        <v>23.414999999999999</v>
       </c>
       <c r="C59">
         <v>0.56000000000000005</v>
       </c>
       <c r="D59">
-        <v>27.952999999999999</v>
+        <v>56.030999999999999</v>
       </c>
       <c r="E59">
         <v>0.56000000000000005</v>
       </c>
       <c r="F59">
-        <v>77.521000000000001</v>
+        <v>156.054</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -5136,19 +5136,19 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="B60">
-        <v>11.776</v>
+        <v>23.513000000000002</v>
       </c>
       <c r="C60">
         <v>0.56999999999999995</v>
       </c>
       <c r="D60">
-        <v>27.885999999999999</v>
+        <v>55.56</v>
       </c>
       <c r="E60">
         <v>0.56999999999999995</v>
       </c>
       <c r="F60">
-        <v>78.340999999999994</v>
+        <v>156.27600000000001</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -5156,19 +5156,19 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="B61">
-        <v>11.722</v>
+        <v>23.414999999999999</v>
       </c>
       <c r="C61">
         <v>0.57999999999999996</v>
       </c>
       <c r="D61">
-        <v>27.783000000000001</v>
+        <v>55.35</v>
       </c>
       <c r="E61">
         <v>0.57999999999999996</v>
       </c>
       <c r="F61">
-        <v>77.540999999999997</v>
+        <v>154.97499999999999</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -5176,19 +5176,19 @@
         <v>0.59</v>
       </c>
       <c r="B62">
-        <v>11.69</v>
+        <v>23.297000000000001</v>
       </c>
       <c r="C62">
         <v>0.59</v>
       </c>
       <c r="D62">
-        <v>28.097000000000001</v>
+        <v>55.140999999999998</v>
       </c>
       <c r="E62">
         <v>0.59</v>
       </c>
       <c r="F62">
-        <v>77.367000000000004</v>
+        <v>155.04300000000001</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5196,19 +5196,19 @@
         <v>0.6</v>
       </c>
       <c r="B63">
-        <v>11.726000000000001</v>
+        <v>23.454000000000001</v>
       </c>
       <c r="C63">
         <v>0.6</v>
       </c>
       <c r="D63">
-        <v>28.052</v>
+        <v>54.795000000000002</v>
       </c>
       <c r="E63">
         <v>0.6</v>
       </c>
       <c r="F63">
-        <v>77.183999999999997</v>
+        <v>156.61500000000001</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5216,19 +5216,19 @@
         <v>0.61</v>
       </c>
       <c r="B64">
-        <v>11.728</v>
+        <v>23.507000000000001</v>
       </c>
       <c r="C64">
         <v>0.61</v>
       </c>
       <c r="D64">
-        <v>27.78</v>
+        <v>54.843000000000004</v>
       </c>
       <c r="E64">
         <v>0.61</v>
       </c>
       <c r="F64">
-        <v>76.927000000000007</v>
+        <v>155.79900000000001</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5236,19 +5236,19 @@
         <v>0.62</v>
       </c>
       <c r="B65">
-        <v>11.813000000000001</v>
+        <v>23.323</v>
       </c>
       <c r="C65">
         <v>0.62</v>
       </c>
       <c r="D65">
-        <v>27.948</v>
+        <v>55.36</v>
       </c>
       <c r="E65">
         <v>0.62</v>
       </c>
       <c r="F65">
-        <v>77.509</v>
+        <v>153.381</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5256,19 +5256,19 @@
         <v>0.63</v>
       </c>
       <c r="B66">
-        <v>11.79</v>
+        <v>23.606000000000002</v>
       </c>
       <c r="C66">
         <v>0.63</v>
       </c>
       <c r="D66">
-        <v>27.425000000000001</v>
+        <v>55.170999999999999</v>
       </c>
       <c r="E66">
         <v>0.63</v>
       </c>
       <c r="F66">
-        <v>77.734999999999999</v>
+        <v>154.63800000000001</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5276,19 +5276,19 @@
         <v>0.64</v>
       </c>
       <c r="B67">
-        <v>11.657</v>
+        <v>23.484999999999999</v>
       </c>
       <c r="C67">
         <v>0.64</v>
       </c>
       <c r="D67">
-        <v>27.858000000000001</v>
+        <v>54.906999999999996</v>
       </c>
       <c r="E67">
         <v>0.64</v>
       </c>
       <c r="F67">
-        <v>77.352000000000004</v>
+        <v>155.494</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5296,19 +5296,19 @@
         <v>0.65</v>
       </c>
       <c r="B68">
-        <v>11.682</v>
+        <v>23.331</v>
       </c>
       <c r="C68">
         <v>0.65</v>
       </c>
       <c r="D68">
-        <v>27.672000000000001</v>
+        <v>55.45</v>
       </c>
       <c r="E68">
         <v>0.65</v>
       </c>
       <c r="F68">
-        <v>77.114999999999995</v>
+        <v>155.24299999999999</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5316,19 +5316,19 @@
         <v>0.66</v>
       </c>
       <c r="B69">
-        <v>11.692</v>
+        <v>23.3</v>
       </c>
       <c r="C69">
         <v>0.66</v>
       </c>
       <c r="D69">
-        <v>27.629000000000001</v>
+        <v>55.515000000000001</v>
       </c>
       <c r="E69">
         <v>0.66</v>
       </c>
       <c r="F69">
-        <v>77.912999999999997</v>
+        <v>156.40100000000001</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -5336,19 +5336,19 @@
         <v>0.67</v>
       </c>
       <c r="B70">
-        <v>11.683999999999999</v>
+        <v>23.43</v>
       </c>
       <c r="C70">
         <v>0.67</v>
       </c>
       <c r="D70">
-        <v>27.611999999999998</v>
+        <v>55.332000000000001</v>
       </c>
       <c r="E70">
         <v>0.67</v>
       </c>
       <c r="F70">
-        <v>77.81</v>
+        <v>156.21799999999999</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -5356,19 +5356,19 @@
         <v>0.68</v>
       </c>
       <c r="B71">
-        <v>11.71</v>
+        <v>23.515999999999998</v>
       </c>
       <c r="C71">
         <v>0.68</v>
       </c>
       <c r="D71">
-        <v>27.858000000000001</v>
+        <v>55.84</v>
       </c>
       <c r="E71">
         <v>0.68</v>
       </c>
       <c r="F71">
-        <v>77.171000000000006</v>
+        <v>154.94300000000001</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5376,19 +5376,19 @@
         <v>0.69</v>
       </c>
       <c r="B72">
-        <v>11.888999999999999</v>
+        <v>23.14</v>
       </c>
       <c r="C72">
         <v>0.69</v>
       </c>
       <c r="D72">
-        <v>27.946999999999999</v>
+        <v>55.21</v>
       </c>
       <c r="E72">
         <v>0.69</v>
       </c>
       <c r="F72">
-        <v>77.566999999999993</v>
+        <v>154.10599999999999</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5396,19 +5396,19 @@
         <v>0.7</v>
       </c>
       <c r="B73">
-        <v>11.757999999999999</v>
+        <v>23.763999999999999</v>
       </c>
       <c r="C73">
         <v>0.7</v>
       </c>
       <c r="D73">
-        <v>27.696000000000002</v>
+        <v>54.838000000000001</v>
       </c>
       <c r="E73">
         <v>0.7</v>
       </c>
       <c r="F73">
-        <v>77.367999999999995</v>
+        <v>155.08099999999999</v>
       </c>
     </row>
   </sheetData>
@@ -5423,7 +5423,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5464,19 +5464,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>22.748000000000001</v>
+        <v>43.454000000000001</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>85.347999999999999</v>
+        <v>177.053</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>425.69099999999997</v>
+        <v>1046.684</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5484,19 +5484,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>11.292</v>
+        <v>22.338999999999999</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
       </c>
       <c r="D4" s="4">
-        <v>28.364999999999998</v>
+        <v>62.835999999999999</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
       </c>
       <c r="F4" s="4">
-        <v>87.13</v>
+        <v>223.1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5504,19 +5504,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>10.050000000000001</v>
+        <v>19.768000000000001</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
       </c>
       <c r="D5" s="4">
-        <v>23.452000000000002</v>
+        <v>48.167999999999999</v>
       </c>
       <c r="E5" s="4">
         <v>3</v>
       </c>
       <c r="F5" s="4">
-        <v>67.478999999999999</v>
+        <v>158.041</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5524,19 +5524,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>9.43</v>
+        <v>18.603999999999999</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>21.56</v>
+        <v>43.064999999999998</v>
       </c>
       <c r="E6" s="4">
         <v>4</v>
       </c>
       <c r="F6" s="4">
-        <v>60.908999999999999</v>
+        <v>135.417</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5544,19 +5544,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>9.3819999999999997</v>
+        <v>18.466999999999999</v>
       </c>
       <c r="C7" s="4">
         <v>5</v>
       </c>
       <c r="D7" s="4">
-        <v>20.533999999999999</v>
+        <v>41.371000000000002</v>
       </c>
       <c r="E7" s="4">
         <v>5</v>
       </c>
       <c r="F7" s="4">
-        <v>57.137</v>
+        <v>124.072</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5564,19 +5564,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>9.1829999999999998</v>
+        <v>18.213000000000001</v>
       </c>
       <c r="C8" s="4">
         <v>6</v>
       </c>
       <c r="D8" s="4">
-        <v>20.015000000000001</v>
+        <v>39.871000000000002</v>
       </c>
       <c r="E8" s="4">
         <v>6</v>
       </c>
       <c r="F8" s="4">
-        <v>55.398000000000003</v>
+        <v>116.199</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5584,13 +5584,13 @@
         <v>7</v>
       </c>
       <c r="D9" s="4">
-        <v>19.579000000000001</v>
+        <v>39.209000000000003</v>
       </c>
       <c r="E9" s="4">
         <v>7</v>
       </c>
       <c r="F9" s="4">
-        <v>54.082999999999998</v>
+        <v>111.149</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5598,13 +5598,13 @@
         <v>8</v>
       </c>
       <c r="D10" s="4">
-        <v>19.459</v>
+        <v>38.743000000000002</v>
       </c>
       <c r="E10" s="4">
         <v>8</v>
       </c>
       <c r="F10" s="4">
-        <v>52.863</v>
+        <v>107.60299999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5612,13 +5612,13 @@
         <v>9</v>
       </c>
       <c r="D11" s="4">
-        <v>19.387</v>
+        <v>38.393999999999998</v>
       </c>
       <c r="E11" s="4">
         <v>9</v>
       </c>
       <c r="F11" s="4">
-        <v>52.009</v>
+        <v>106.495</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5626,13 +5626,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="4">
-        <v>19.239000000000001</v>
+        <v>38.079000000000001</v>
       </c>
       <c r="E12" s="4">
         <v>10</v>
       </c>
       <c r="F12" s="4">
-        <v>51.343000000000004</v>
+        <v>104.836</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5640,13 +5640,13 @@
         <v>11</v>
       </c>
       <c r="D13" s="4">
-        <v>19.222999999999999</v>
+        <v>38.073</v>
       </c>
       <c r="E13" s="4">
         <v>11</v>
       </c>
       <c r="F13" s="4">
-        <v>51.411999999999999</v>
+        <v>102.304</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5654,13 +5654,13 @@
         <v>12</v>
       </c>
       <c r="D14" s="4">
-        <v>19.268000000000001</v>
+        <v>38.195</v>
       </c>
       <c r="E14" s="4">
         <v>12</v>
       </c>
       <c r="F14" s="4">
-        <v>50.685000000000002</v>
+        <v>101.749</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5668,7 +5668,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="4">
-        <v>50.247</v>
+        <v>101.8</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5676,7 +5676,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="4">
-        <v>50.475000000000001</v>
+        <v>100.89</v>
       </c>
     </row>
     <row r="17" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5684,7 +5684,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="4">
-        <v>50.279000000000003</v>
+        <v>99.393000000000001</v>
       </c>
     </row>
     <row r="18" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5692,7 +5692,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="4">
-        <v>49.686999999999998</v>
+        <v>99.561000000000007</v>
       </c>
     </row>
     <row r="19" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5700,7 +5700,7 @@
         <v>17</v>
       </c>
       <c r="F19" s="4">
-        <v>49.825000000000003</v>
+        <v>99.171000000000006</v>
       </c>
     </row>
     <row r="20" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5708,7 +5708,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="4">
-        <v>49.368000000000002</v>
+        <v>99.74</v>
       </c>
     </row>
     <row r="21" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5716,7 +5716,7 @@
         <v>19</v>
       </c>
       <c r="F21" s="4">
-        <v>50.161000000000001</v>
+        <v>100.456</v>
       </c>
     </row>
     <row r="22" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5724,7 +5724,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="4">
-        <v>49.887</v>
+        <v>98.298000000000002</v>
       </c>
     </row>
     <row r="23" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5732,7 +5732,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="4">
-        <v>49.026000000000003</v>
+        <v>97.942999999999998</v>
       </c>
     </row>
     <row r="24" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5740,7 +5740,7 @@
         <v>22</v>
       </c>
       <c r="F24" s="4">
-        <v>49.786000000000001</v>
+        <v>98.296000000000006</v>
       </c>
     </row>
     <row r="25" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5748,7 +5748,7 @@
         <v>23</v>
       </c>
       <c r="F25" s="4">
-        <v>49.621000000000002</v>
+        <v>97.86</v>
       </c>
     </row>
     <row r="26" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5756,7 +5756,7 @@
         <v>24</v>
       </c>
       <c r="F26" s="4">
-        <v>49.02</v>
+        <v>98.747</v>
       </c>
     </row>
     <row r="27" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5764,7 +5764,7 @@
         <v>25</v>
       </c>
       <c r="F27" s="4">
-        <v>48.896000000000001</v>
+        <v>98.882000000000005</v>
       </c>
     </row>
     <row r="28" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5772,7 +5772,7 @@
         <v>26</v>
       </c>
       <c r="F28" s="4">
-        <v>49.277999999999999</v>
+        <v>98.867999999999995</v>
       </c>
     </row>
     <row r="29" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5780,7 +5780,7 @@
         <v>27</v>
       </c>
       <c r="F29" s="4">
-        <v>48.723999999999997</v>
+        <v>98.418000000000006</v>
       </c>
     </row>
     <row r="30" spans="5:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5788,7 +5788,7 @@
         <v>28</v>
       </c>
       <c r="F30" s="4">
-        <v>49.165999999999997</v>
+        <v>98.569000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>